<commit_message>
Update stats template to add notes
</commit_message>
<xml_diff>
--- a/scripts/cli/authority_stats.xlsx
+++ b/scripts/cli/authority_stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -13,18 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Standard report" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -183,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -259,6 +250,12 @@
   <si>
     <t>The full data associated with any shortlinks can be viewed by clicking  the link below and then scrolling to the appropriate shortlink.</t>
   </si>
+  <si>
+    <t>Current total number of Freeglers</t>
+  </si>
+  <si>
+    <t>Calculated using WRAP's Benefits of Reuse tool.</t>
+  </si>
 </sst>
 </file>
 
@@ -270,7 +267,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +490,26 @@
       <i/>
       <sz val="9"/>
       <color rgb="FF0070C0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -727,7 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -833,6 +850,20 @@
     <xf numFmtId="166" fontId="25" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,17 +885,6 @@
     <xf numFmtId="0" fontId="29" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent" xfId="7"/>
@@ -1256,7 +1276,7 @@
   <dimension ref="A1:AMR561"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+      <selection activeCell="N18" sqref="N18:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1674,12 +1694,12 @@
     </row>
     <row r="7" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -7892,10 +7912,10 @@
       <c r="A13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="66"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="59"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -10058,36 +10078,36 @@
     </row>
     <row r="18" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A18" s="32"/>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="62" t="s">
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="57" t="s">
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="57" t="s">
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="O18" s="57"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="57" t="s">
+      <c r="O18" s="65"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="S18" s="57"/>
-      <c r="T18" s="57"/>
-      <c r="U18" s="58"/>
+      <c r="S18" s="65"/>
+      <c r="T18" s="65"/>
+      <c r="U18" s="66"/>
     </row>
     <row r="19" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
@@ -10170,10 +10190,10 @@
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
       <c r="M20" s="39"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="67"/>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="68"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="61"/>
       <c r="R20" s="38"/>
       <c r="S20" s="38"/>
       <c r="T20" s="38"/>
@@ -44441,4 +44461,49 @@
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.25" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.25" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Improvements to authority stats
</commit_message>
<xml_diff>
--- a/scripts/cli/authority_stats.xlsx
+++ b/scripts/cli/authority_stats.xlsx
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>xxx Freegle</t>
   </si>
   <si>
     <t>CO2 saved (tonnes)</t>
@@ -588,7 +585,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -698,19 +695,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -749,7 +733,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -811,9 +795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,8 +835,6 @@
     <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -877,6 +856,7 @@
     <xf numFmtId="0" fontId="28" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -898,7 +878,6 @@
     <xf numFmtId="0" fontId="29" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent" xfId="7"/>
@@ -1287,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMR562"/>
+  <dimension ref="A1:AMR563"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1304,7 +1283,7 @@
   <sheetData>
     <row r="1" spans="1:1032" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
@@ -1708,12 +1687,12 @@
     </row>
     <row r="7" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="73"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -5850,12 +5829,12 @@
     </row>
     <row r="11" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="52"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -6888,10 +6867,10 @@
       <c r="A12" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="55"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -7922,12 +7901,12 @@
     </row>
     <row r="13" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="51"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:1032" x14ac:dyDescent="0.3">
@@ -9054,40 +9033,40 @@
     </row>
     <row r="17" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="74" t="s">
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="69" t="s">
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="69" t="s">
+      <c r="S17" s="65"/>
+      <c r="T17" s="65"/>
+      <c r="U17" s="66"/>
+    </row>
+    <row r="18" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A18" s="63" t="s">
         <v>12</v>
-      </c>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="70"/>
-    </row>
-    <row r="18" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A18" s="68" t="s">
-        <v>13</v>
       </c>
       <c r="B18" s="31">
         <v>43466</v>
@@ -9150,10 +9129,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
-        <v>10</v>
-      </c>
+    <row r="19" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
@@ -9162,41 +9139,97 @@
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
       <c r="I19" s="36"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="57"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="36"/>
       <c r="R19" s="35"/>
       <c r="S19" s="35"/>
       <c r="T19" s="35"/>
       <c r="U19" s="36"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="15"/>
+      <c r="AM19" s="15"/>
+      <c r="AN19" s="15"/>
+      <c r="AO19" s="15"/>
+      <c r="AP19" s="15"/>
+      <c r="AQ19" s="15"/>
+      <c r="AR19" s="15"/>
+      <c r="AS19" s="15"/>
+      <c r="AT19" s="15"/>
+      <c r="AU19" s="15"/>
+      <c r="AV19" s="15"/>
+      <c r="AW19" s="15"/>
+      <c r="AX19" s="15"/>
+      <c r="AY19" s="15"/>
+      <c r="AZ19" s="15"/>
+      <c r="BA19" s="15"/>
+      <c r="BB19" s="15"/>
+      <c r="BC19" s="15"/>
+      <c r="BD19" s="15"/>
+      <c r="BE19" s="15"/>
+      <c r="BF19" s="15"/>
+      <c r="BG19" s="15"/>
+      <c r="BH19" s="15"/>
+      <c r="BI19" s="15"/>
+      <c r="BJ19" s="15"/>
+      <c r="BK19" s="15"/>
+      <c r="BL19" s="15"/>
+      <c r="BM19" s="15"/>
+      <c r="BN19" s="15"/>
+      <c r="BO19" s="15"/>
+      <c r="BP19" s="15"/>
+      <c r="BQ19" s="15"/>
+      <c r="BR19" s="15"/>
+      <c r="BS19" s="15"/>
+      <c r="BT19" s="15"/>
+      <c r="BU19" s="15"/>
+      <c r="BV19" s="15"/>
+      <c r="BW19" s="15"/>
+      <c r="BX19" s="15"/>
+      <c r="BY19" s="15"/>
     </row>
     <row r="20" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="39"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
       <c r="AD20" s="15"/>
       <c r="AE20" s="15"/>
       <c r="AF20" s="15"/>
@@ -9246,40 +9279,44 @@
       <c r="BX20" s="15"/>
       <c r="BY20" s="15"/>
     </row>
-    <row r="21" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="17"/>
-      <c r="Y21" s="18"/>
+    <row r="21" spans="1:1032" s="39" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A21" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
       <c r="Z21" s="15"/>
       <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
+      <c r="AB21" s="19"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
       <c r="AE21" s="15"/>
       <c r="AF21" s="15"/>
-      <c r="AG21" s="15"/>
+      <c r="AG21" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="AH21" s="15"/>
       <c r="AI21" s="15"/>
       <c r="AJ21" s="15"/>
@@ -9325,17 +9362,15 @@
       <c r="BX21" s="15"/>
       <c r="BY21" s="15"/>
     </row>
-    <row r="22" spans="1:1032" s="42" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
+    <row r="22" spans="1:1032" s="39" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
@@ -9360,9 +9395,7 @@
       <c r="AD22" s="15"/>
       <c r="AE22" s="15"/>
       <c r="AF22" s="15"/>
-      <c r="AG22" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="AG22" s="15"/>
       <c r="AH22" s="15"/>
       <c r="AI22" s="15"/>
       <c r="AJ22" s="15"/>
@@ -9408,12 +9441,14 @@
       <c r="BX22" s="15"/>
       <c r="BY22" s="15"/>
     </row>
-    <row r="23" spans="1:1032" s="42" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+    <row r="23" spans="1:1032" s="39" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A23" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -9487,14 +9522,20 @@
       <c r="BX23" s="15"/>
       <c r="BY23" s="15"/>
     </row>
-    <row r="24" spans="1:1032" s="42" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A24" s="61" t="s">
-        <v>8</v>
+    <row r="24" spans="1:1032" s="40" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A24" s="64"/>
+      <c r="B24" s="62">
+        <v>43466</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="C24" s="57">
+        <v>43497</v>
+      </c>
+      <c r="D24" s="57">
+        <v>43525</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
@@ -9515,13 +9556,13 @@
       <c r="W24" s="19"/>
       <c r="X24" s="19"/>
       <c r="Y24" s="19"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="15"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="19"/>
       <c r="AB24" s="19"/>
-      <c r="AC24" s="15"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15"/>
-      <c r="AF24" s="15"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
       <c r="AG24" s="15"/>
       <c r="AH24" s="15"/>
       <c r="AI24" s="15"/>
@@ -9568,47 +9609,12 @@
       <c r="BX24" s="15"/>
       <c r="BY24" s="15"/>
     </row>
-    <row r="25" spans="1:1032" s="43" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A25" s="76"/>
-      <c r="B25" s="67">
-        <v>43466</v>
-      </c>
-      <c r="C25" s="62">
-        <v>43497</v>
-      </c>
-      <c r="D25" s="62">
-        <v>43525</v>
-      </c>
-      <c r="E25" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="19"/>
-      <c r="AF25" s="19"/>
+    <row r="25" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="61"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="15"/>
       <c r="AI25" s="15"/>
@@ -9656,11 +9662,11 @@
       <c r="BY25" s="15"/>
     </row>
     <row r="26" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A26" s="64"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="66"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
       <c r="AG26" s="15"/>
       <c r="AH26" s="15"/>
       <c r="AI26" s="15"/>
@@ -9708,10 +9714,11 @@
       <c r="BY26" s="15"/>
     </row>
     <row r="27" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
       <c r="AG27" s="15"/>
       <c r="AH27" s="15"/>
       <c r="AI27" s="15"/>
@@ -9758,41 +9765,11 @@
       <c r="BX27" s="15"/>
       <c r="BY27" s="15"/>
     </row>
-    <row r="28" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A28" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="19"/>
-      <c r="Y28" s="19"/>
-      <c r="Z28" s="19"/>
-      <c r="AA28" s="19"/>
-      <c r="AB28" s="19"/>
-      <c r="AC28" s="19"/>
-      <c r="AD28" s="19"/>
-      <c r="AE28" s="19"/>
-      <c r="AF28" s="19"/>
+    <row r="28" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
       <c r="AG28" s="15"/>
       <c r="AH28" s="15"/>
       <c r="AI28" s="15"/>
@@ -9838,993 +9815,38 @@
       <c r="BW28" s="15"/>
       <c r="BX28" s="15"/>
       <c r="BY28" s="15"/>
-      <c r="BZ28" s="19"/>
-      <c r="CA28" s="19"/>
-      <c r="CB28" s="19"/>
-      <c r="CC28" s="19"/>
-      <c r="CD28" s="19"/>
-      <c r="CE28" s="19"/>
-      <c r="CF28" s="19"/>
-      <c r="CG28" s="19"/>
-      <c r="CH28" s="19"/>
-      <c r="CI28" s="19"/>
-      <c r="CJ28" s="19"/>
-      <c r="CK28" s="19"/>
-      <c r="CL28" s="19"/>
-      <c r="CM28" s="19"/>
-      <c r="CN28" s="19"/>
-      <c r="CO28" s="19"/>
-      <c r="CP28" s="19"/>
-      <c r="CQ28" s="19"/>
-      <c r="CR28" s="19"/>
-      <c r="CS28" s="19"/>
-      <c r="CT28" s="19"/>
-      <c r="CU28" s="19"/>
-      <c r="CV28" s="19"/>
-      <c r="CW28" s="19"/>
-      <c r="CX28" s="19"/>
-      <c r="CY28" s="19"/>
-      <c r="CZ28" s="19"/>
-      <c r="DA28" s="19"/>
-      <c r="DB28" s="19"/>
-      <c r="DC28" s="19"/>
-      <c r="DD28" s="19"/>
-      <c r="DE28" s="19"/>
-      <c r="DF28" s="19"/>
-      <c r="DG28" s="19"/>
-      <c r="DH28" s="19"/>
-      <c r="DI28" s="19"/>
-      <c r="DJ28" s="19"/>
-      <c r="DK28" s="19"/>
-      <c r="DL28" s="19"/>
-      <c r="DM28" s="19"/>
-      <c r="DN28" s="19"/>
-      <c r="DO28" s="19"/>
-      <c r="DP28" s="19"/>
-      <c r="DQ28" s="19"/>
-      <c r="DR28" s="19"/>
-      <c r="DS28" s="19"/>
-      <c r="DT28" s="19"/>
-      <c r="DU28" s="19"/>
-      <c r="DV28" s="19"/>
-      <c r="DW28" s="19"/>
-      <c r="DX28" s="19"/>
-      <c r="DY28" s="19"/>
-      <c r="DZ28" s="19"/>
-      <c r="EA28" s="19"/>
-      <c r="EB28" s="19"/>
-      <c r="EC28" s="19"/>
-      <c r="ED28" s="19"/>
-      <c r="EE28" s="19"/>
-      <c r="EF28" s="19"/>
-      <c r="EG28" s="19"/>
-      <c r="EH28" s="19"/>
-      <c r="EI28" s="19"/>
-      <c r="EJ28" s="19"/>
-      <c r="EK28" s="19"/>
-      <c r="EL28" s="19"/>
-      <c r="EM28" s="19"/>
-      <c r="EN28" s="19"/>
-      <c r="EO28" s="19"/>
-      <c r="EP28" s="19"/>
-      <c r="EQ28" s="19"/>
-      <c r="ER28" s="19"/>
-      <c r="ES28" s="19"/>
-      <c r="ET28" s="19"/>
-      <c r="EU28" s="19"/>
-      <c r="EV28" s="19"/>
-      <c r="EW28" s="19"/>
-      <c r="EX28" s="19"/>
-      <c r="EY28" s="19"/>
-      <c r="EZ28" s="19"/>
-      <c r="FA28" s="19"/>
-      <c r="FB28" s="19"/>
-      <c r="FC28" s="19"/>
-      <c r="FD28" s="19"/>
-      <c r="FE28" s="19"/>
-      <c r="FF28" s="19"/>
-      <c r="FG28" s="19"/>
-      <c r="FH28" s="19"/>
-      <c r="FI28" s="19"/>
-      <c r="FJ28" s="19"/>
-      <c r="FK28" s="19"/>
-      <c r="FL28" s="19"/>
-      <c r="FM28" s="19"/>
-      <c r="FN28" s="19"/>
-      <c r="FO28" s="19"/>
-      <c r="FP28" s="19"/>
-      <c r="FQ28" s="19"/>
-      <c r="FR28" s="19"/>
-      <c r="FS28" s="19"/>
-      <c r="FT28" s="19"/>
-      <c r="FU28" s="19"/>
-      <c r="FV28" s="19"/>
-      <c r="FW28" s="19"/>
-      <c r="FX28" s="19"/>
-      <c r="FY28" s="19"/>
-      <c r="FZ28" s="19"/>
-      <c r="GA28" s="19"/>
-      <c r="GB28" s="19"/>
-      <c r="GC28" s="19"/>
-      <c r="GD28" s="19"/>
-      <c r="GE28" s="19"/>
-      <c r="GF28" s="19"/>
-      <c r="GG28" s="19"/>
-      <c r="GH28" s="19"/>
-      <c r="GI28" s="19"/>
-      <c r="GJ28" s="19"/>
-      <c r="GK28" s="19"/>
-      <c r="GL28" s="19"/>
-      <c r="GM28" s="19"/>
-      <c r="GN28" s="19"/>
-      <c r="GO28" s="19"/>
-      <c r="GP28" s="19"/>
-      <c r="GQ28" s="19"/>
-      <c r="GR28" s="19"/>
-      <c r="GS28" s="19"/>
-      <c r="GT28" s="19"/>
-      <c r="GU28" s="19"/>
-      <c r="GV28" s="19"/>
-      <c r="GW28" s="19"/>
-      <c r="GX28" s="19"/>
-      <c r="GY28" s="19"/>
-      <c r="GZ28" s="19"/>
-      <c r="HA28" s="19"/>
-      <c r="HB28" s="19"/>
-      <c r="HC28" s="19"/>
-      <c r="HD28" s="19"/>
-      <c r="HE28" s="19"/>
-      <c r="HF28" s="19"/>
-      <c r="HG28" s="19"/>
-      <c r="HH28" s="19"/>
-      <c r="HI28" s="19"/>
-      <c r="HJ28" s="19"/>
-      <c r="HK28" s="19"/>
-      <c r="HL28" s="19"/>
-      <c r="HM28" s="19"/>
-      <c r="HN28" s="19"/>
-      <c r="HO28" s="19"/>
-      <c r="HP28" s="19"/>
-      <c r="HQ28" s="19"/>
-      <c r="HR28" s="19"/>
-      <c r="HS28" s="19"/>
-      <c r="HT28" s="19"/>
-      <c r="HU28" s="19"/>
-      <c r="HV28" s="19"/>
-      <c r="HW28" s="19"/>
-      <c r="HX28" s="19"/>
-      <c r="HY28" s="19"/>
-      <c r="HZ28" s="19"/>
-      <c r="IA28" s="19"/>
-      <c r="IB28" s="19"/>
-      <c r="IC28" s="19"/>
-      <c r="ID28" s="19"/>
-      <c r="IE28" s="19"/>
-      <c r="IF28" s="19"/>
-      <c r="IG28" s="19"/>
-      <c r="IH28" s="19"/>
-      <c r="II28" s="19"/>
-      <c r="IJ28" s="19"/>
-      <c r="IK28" s="19"/>
-      <c r="IL28" s="19"/>
-      <c r="IM28" s="19"/>
-      <c r="IN28" s="19"/>
-      <c r="IO28" s="19"/>
-      <c r="IP28" s="19"/>
-      <c r="IQ28" s="19"/>
-      <c r="IR28" s="19"/>
-      <c r="IS28" s="19"/>
-      <c r="IT28" s="19"/>
-      <c r="IU28" s="19"/>
-      <c r="IV28" s="19"/>
-      <c r="IW28" s="19"/>
-      <c r="IX28" s="19"/>
-      <c r="IY28" s="19"/>
-      <c r="IZ28" s="19"/>
-      <c r="JA28" s="19"/>
-      <c r="JB28" s="19"/>
-      <c r="JC28" s="19"/>
-      <c r="JD28" s="19"/>
-      <c r="JE28" s="19"/>
-      <c r="JF28" s="19"/>
-      <c r="JG28" s="19"/>
-      <c r="JH28" s="19"/>
-      <c r="JI28" s="19"/>
-      <c r="JJ28" s="19"/>
-      <c r="JK28" s="19"/>
-      <c r="JL28" s="19"/>
-      <c r="JM28" s="19"/>
-      <c r="JN28" s="19"/>
-      <c r="JO28" s="19"/>
-      <c r="JP28" s="19"/>
-      <c r="JQ28" s="19"/>
-      <c r="JR28" s="19"/>
-      <c r="JS28" s="19"/>
-      <c r="JT28" s="19"/>
-      <c r="JU28" s="19"/>
-      <c r="JV28" s="19"/>
-      <c r="JW28" s="19"/>
-      <c r="JX28" s="19"/>
-      <c r="JY28" s="19"/>
-      <c r="JZ28" s="19"/>
-      <c r="KA28" s="19"/>
-      <c r="KB28" s="19"/>
-      <c r="KC28" s="19"/>
-      <c r="KD28" s="19"/>
-      <c r="KE28" s="19"/>
-      <c r="KF28" s="19"/>
-      <c r="KG28" s="19"/>
-      <c r="KH28" s="19"/>
-      <c r="KI28" s="19"/>
-      <c r="KJ28" s="19"/>
-      <c r="KK28" s="19"/>
-      <c r="KL28" s="19"/>
-      <c r="KM28" s="19"/>
-      <c r="KN28" s="19"/>
-      <c r="KO28" s="19"/>
-      <c r="KP28" s="19"/>
-      <c r="KQ28" s="19"/>
-      <c r="KR28" s="19"/>
-      <c r="KS28" s="19"/>
-      <c r="KT28" s="19"/>
-      <c r="KU28" s="19"/>
-      <c r="KV28" s="19"/>
-      <c r="KW28" s="19"/>
-      <c r="KX28" s="19"/>
-      <c r="KY28" s="19"/>
-      <c r="KZ28" s="19"/>
-      <c r="LA28" s="19"/>
-      <c r="LB28" s="19"/>
-      <c r="LC28" s="19"/>
-      <c r="LD28" s="19"/>
-      <c r="LE28" s="19"/>
-      <c r="LF28" s="19"/>
-      <c r="LG28" s="19"/>
-      <c r="LH28" s="19"/>
-      <c r="LI28" s="19"/>
-      <c r="LJ28" s="19"/>
-      <c r="LK28" s="19"/>
-      <c r="LL28" s="19"/>
-      <c r="LM28" s="19"/>
-      <c r="LN28" s="19"/>
-      <c r="LO28" s="19"/>
-      <c r="LP28" s="19"/>
-      <c r="LQ28" s="19"/>
-      <c r="LR28" s="19"/>
-      <c r="LS28" s="19"/>
-      <c r="LT28" s="19"/>
-      <c r="LU28" s="19"/>
-      <c r="LV28" s="19"/>
-      <c r="LW28" s="19"/>
-      <c r="LX28" s="19"/>
-      <c r="LY28" s="19"/>
-      <c r="LZ28" s="19"/>
-      <c r="MA28" s="19"/>
-      <c r="MB28" s="19"/>
-      <c r="MC28" s="19"/>
-      <c r="MD28" s="19"/>
-      <c r="ME28" s="19"/>
-      <c r="MF28" s="19"/>
-      <c r="MG28" s="19"/>
-      <c r="MH28" s="19"/>
-      <c r="MI28" s="19"/>
-      <c r="MJ28" s="19"/>
-      <c r="MK28" s="19"/>
-      <c r="ML28" s="19"/>
-      <c r="MM28" s="19"/>
-      <c r="MN28" s="19"/>
-      <c r="MO28" s="19"/>
-      <c r="MP28" s="19"/>
-      <c r="MQ28" s="19"/>
-      <c r="MR28" s="19"/>
-      <c r="MS28" s="19"/>
-      <c r="MT28" s="19"/>
-      <c r="MU28" s="19"/>
-      <c r="MV28" s="19"/>
-      <c r="MW28" s="19"/>
-      <c r="MX28" s="19"/>
-      <c r="MY28" s="19"/>
-      <c r="MZ28" s="19"/>
-      <c r="NA28" s="19"/>
-      <c r="NB28" s="19"/>
-      <c r="NC28" s="19"/>
-      <c r="ND28" s="19"/>
-      <c r="NE28" s="19"/>
-      <c r="NF28" s="19"/>
-      <c r="NG28" s="19"/>
-      <c r="NH28" s="19"/>
-      <c r="NI28" s="19"/>
-      <c r="NJ28" s="19"/>
-      <c r="NK28" s="19"/>
-      <c r="NL28" s="19"/>
-      <c r="NM28" s="19"/>
-      <c r="NN28" s="19"/>
-      <c r="NO28" s="19"/>
-      <c r="NP28" s="19"/>
-      <c r="NQ28" s="19"/>
-      <c r="NR28" s="19"/>
-      <c r="NS28" s="19"/>
-      <c r="NT28" s="19"/>
-      <c r="NU28" s="19"/>
-      <c r="NV28" s="19"/>
-      <c r="NW28" s="19"/>
-      <c r="NX28" s="19"/>
-      <c r="NY28" s="19"/>
-      <c r="NZ28" s="19"/>
-      <c r="OA28" s="19"/>
-      <c r="OB28" s="19"/>
-      <c r="OC28" s="19"/>
-      <c r="OD28" s="19"/>
-      <c r="OE28" s="19"/>
-      <c r="OF28" s="19"/>
-      <c r="OG28" s="19"/>
-      <c r="OH28" s="19"/>
-      <c r="OI28" s="19"/>
-      <c r="OJ28" s="19"/>
-      <c r="OK28" s="19"/>
-      <c r="OL28" s="19"/>
-      <c r="OM28" s="19"/>
-      <c r="ON28" s="19"/>
-      <c r="OO28" s="19"/>
-      <c r="OP28" s="19"/>
-      <c r="OQ28" s="19"/>
-      <c r="OR28" s="19"/>
-      <c r="OS28" s="19"/>
-      <c r="OT28" s="19"/>
-      <c r="OU28" s="19"/>
-      <c r="OV28" s="19"/>
-      <c r="OW28" s="19"/>
-      <c r="OX28" s="19"/>
-      <c r="OY28" s="19"/>
-      <c r="OZ28" s="19"/>
-      <c r="PA28" s="19"/>
-      <c r="PB28" s="19"/>
-      <c r="PC28" s="19"/>
-      <c r="PD28" s="19"/>
-      <c r="PE28" s="19"/>
-      <c r="PF28" s="19"/>
-      <c r="PG28" s="19"/>
-      <c r="PH28" s="19"/>
-      <c r="PI28" s="19"/>
-      <c r="PJ28" s="19"/>
-      <c r="PK28" s="19"/>
-      <c r="PL28" s="19"/>
-      <c r="PM28" s="19"/>
-      <c r="PN28" s="19"/>
-      <c r="PO28" s="19"/>
-      <c r="PP28" s="19"/>
-      <c r="PQ28" s="19"/>
-      <c r="PR28" s="19"/>
-      <c r="PS28" s="19"/>
-      <c r="PT28" s="19"/>
-      <c r="PU28" s="19"/>
-      <c r="PV28" s="19"/>
-      <c r="PW28" s="19"/>
-      <c r="PX28" s="19"/>
-      <c r="PY28" s="19"/>
-      <c r="PZ28" s="19"/>
-      <c r="QA28" s="19"/>
-      <c r="QB28" s="19"/>
-      <c r="QC28" s="19"/>
-      <c r="QD28" s="19"/>
-      <c r="QE28" s="19"/>
-      <c r="QF28" s="19"/>
-      <c r="QG28" s="19"/>
-      <c r="QH28" s="19"/>
-      <c r="QI28" s="19"/>
-      <c r="QJ28" s="19"/>
-      <c r="QK28" s="19"/>
-      <c r="QL28" s="19"/>
-      <c r="QM28" s="19"/>
-      <c r="QN28" s="19"/>
-      <c r="QO28" s="19"/>
-      <c r="QP28" s="19"/>
-      <c r="QQ28" s="19"/>
-      <c r="QR28" s="19"/>
-      <c r="QS28" s="19"/>
-      <c r="QT28" s="19"/>
-      <c r="QU28" s="19"/>
-      <c r="QV28" s="19"/>
-      <c r="QW28" s="19"/>
-      <c r="QX28" s="19"/>
-      <c r="QY28" s="19"/>
-      <c r="QZ28" s="19"/>
-      <c r="RA28" s="19"/>
-      <c r="RB28" s="19"/>
-      <c r="RC28" s="19"/>
-      <c r="RD28" s="19"/>
-      <c r="RE28" s="19"/>
-      <c r="RF28" s="19"/>
-      <c r="RG28" s="19"/>
-      <c r="RH28" s="19"/>
-      <c r="RI28" s="19"/>
-      <c r="RJ28" s="19"/>
-      <c r="RK28" s="19"/>
-      <c r="RL28" s="19"/>
-      <c r="RM28" s="19"/>
-      <c r="RN28" s="19"/>
-      <c r="RO28" s="19"/>
-      <c r="RP28" s="19"/>
-      <c r="RQ28" s="19"/>
-      <c r="RR28" s="19"/>
-      <c r="RS28" s="19"/>
-      <c r="RT28" s="19"/>
-      <c r="RU28" s="19"/>
-      <c r="RV28" s="19"/>
-      <c r="RW28" s="19"/>
-      <c r="RX28" s="19"/>
-      <c r="RY28" s="19"/>
-      <c r="RZ28" s="19"/>
-      <c r="SA28" s="19"/>
-      <c r="SB28" s="19"/>
-      <c r="SC28" s="19"/>
-      <c r="SD28" s="19"/>
-      <c r="SE28" s="19"/>
-      <c r="SF28" s="19"/>
-      <c r="SG28" s="19"/>
-      <c r="SH28" s="19"/>
-      <c r="SI28" s="19"/>
-      <c r="SJ28" s="19"/>
-      <c r="SK28" s="19"/>
-      <c r="SL28" s="19"/>
-      <c r="SM28" s="19"/>
-      <c r="SN28" s="19"/>
-      <c r="SO28" s="19"/>
-      <c r="SP28" s="19"/>
-      <c r="SQ28" s="19"/>
-      <c r="SR28" s="19"/>
-      <c r="SS28" s="19"/>
-      <c r="ST28" s="19"/>
-      <c r="SU28" s="19"/>
-      <c r="SV28" s="19"/>
-      <c r="SW28" s="19"/>
-      <c r="SX28" s="19"/>
-      <c r="SY28" s="19"/>
-      <c r="SZ28" s="19"/>
-      <c r="TA28" s="19"/>
-      <c r="TB28" s="19"/>
-      <c r="TC28" s="19"/>
-      <c r="TD28" s="19"/>
-      <c r="TE28" s="19"/>
-      <c r="TF28" s="19"/>
-      <c r="TG28" s="19"/>
-      <c r="TH28" s="19"/>
-      <c r="TI28" s="19"/>
-      <c r="TJ28" s="19"/>
-      <c r="TK28" s="19"/>
-      <c r="TL28" s="19"/>
-      <c r="TM28" s="19"/>
-      <c r="TN28" s="19"/>
-      <c r="TO28" s="19"/>
-      <c r="TP28" s="19"/>
-      <c r="TQ28" s="19"/>
-      <c r="TR28" s="19"/>
-      <c r="TS28" s="19"/>
-      <c r="TT28" s="19"/>
-      <c r="TU28" s="19"/>
-      <c r="TV28" s="19"/>
-      <c r="TW28" s="19"/>
-      <c r="TX28" s="19"/>
-      <c r="TY28" s="19"/>
-      <c r="TZ28" s="19"/>
-      <c r="UA28" s="19"/>
-      <c r="UB28" s="19"/>
-      <c r="UC28" s="19"/>
-      <c r="UD28" s="19"/>
-      <c r="UE28" s="19"/>
-      <c r="UF28" s="19"/>
-      <c r="UG28" s="19"/>
-      <c r="UH28" s="19"/>
-      <c r="UI28" s="19"/>
-      <c r="UJ28" s="19"/>
-      <c r="UK28" s="19"/>
-      <c r="UL28" s="19"/>
-      <c r="UM28" s="19"/>
-      <c r="UN28" s="19"/>
-      <c r="UO28" s="19"/>
-      <c r="UP28" s="19"/>
-      <c r="UQ28" s="19"/>
-      <c r="UR28" s="19"/>
-      <c r="US28" s="19"/>
-      <c r="UT28" s="19"/>
-      <c r="UU28" s="19"/>
-      <c r="UV28" s="19"/>
-      <c r="UW28" s="19"/>
-      <c r="UX28" s="19"/>
-      <c r="UY28" s="19"/>
-      <c r="UZ28" s="19"/>
-      <c r="VA28" s="19"/>
-      <c r="VB28" s="19"/>
-      <c r="VC28" s="19"/>
-      <c r="VD28" s="19"/>
-      <c r="VE28" s="19"/>
-      <c r="VF28" s="19"/>
-      <c r="VG28" s="19"/>
-      <c r="VH28" s="19"/>
-      <c r="VI28" s="19"/>
-      <c r="VJ28" s="19"/>
-      <c r="VK28" s="19"/>
-      <c r="VL28" s="19"/>
-      <c r="VM28" s="19"/>
-      <c r="VN28" s="19"/>
-      <c r="VO28" s="19"/>
-      <c r="VP28" s="19"/>
-      <c r="VQ28" s="19"/>
-      <c r="VR28" s="19"/>
-      <c r="VS28" s="19"/>
-      <c r="VT28" s="19"/>
-      <c r="VU28" s="19"/>
-      <c r="VV28" s="19"/>
-      <c r="VW28" s="19"/>
-      <c r="VX28" s="19"/>
-      <c r="VY28" s="19"/>
-      <c r="VZ28" s="19"/>
-      <c r="WA28" s="19"/>
-      <c r="WB28" s="19"/>
-      <c r="WC28" s="19"/>
-      <c r="WD28" s="19"/>
-      <c r="WE28" s="19"/>
-      <c r="WF28" s="19"/>
-      <c r="WG28" s="19"/>
-      <c r="WH28" s="19"/>
-      <c r="WI28" s="19"/>
-      <c r="WJ28" s="19"/>
-      <c r="WK28" s="19"/>
-      <c r="WL28" s="19"/>
-      <c r="WM28" s="19"/>
-      <c r="WN28" s="19"/>
-      <c r="WO28" s="19"/>
-      <c r="WP28" s="19"/>
-      <c r="WQ28" s="19"/>
-      <c r="WR28" s="19"/>
-      <c r="WS28" s="19"/>
-      <c r="WT28" s="19"/>
-      <c r="WU28" s="19"/>
-      <c r="WV28" s="19"/>
-      <c r="WW28" s="19"/>
-      <c r="WX28" s="19"/>
-      <c r="WY28" s="19"/>
-      <c r="WZ28" s="19"/>
-      <c r="XA28" s="19"/>
-      <c r="XB28" s="19"/>
-      <c r="XC28" s="19"/>
-      <c r="XD28" s="19"/>
-      <c r="XE28" s="19"/>
-      <c r="XF28" s="19"/>
-      <c r="XG28" s="19"/>
-      <c r="XH28" s="19"/>
-      <c r="XI28" s="19"/>
-      <c r="XJ28" s="19"/>
-      <c r="XK28" s="19"/>
-      <c r="XL28" s="19"/>
-      <c r="XM28" s="19"/>
-      <c r="XN28" s="19"/>
-      <c r="XO28" s="19"/>
-      <c r="XP28" s="19"/>
-      <c r="XQ28" s="19"/>
-      <c r="XR28" s="19"/>
-      <c r="XS28" s="19"/>
-      <c r="XT28" s="19"/>
-      <c r="XU28" s="19"/>
-      <c r="XV28" s="19"/>
-      <c r="XW28" s="19"/>
-      <c r="XX28" s="19"/>
-      <c r="XY28" s="19"/>
-      <c r="XZ28" s="19"/>
-      <c r="YA28" s="19"/>
-      <c r="YB28" s="19"/>
-      <c r="YC28" s="19"/>
-      <c r="YD28" s="19"/>
-      <c r="YE28" s="19"/>
-      <c r="YF28" s="19"/>
-      <c r="YG28" s="19"/>
-      <c r="YH28" s="19"/>
-      <c r="YI28" s="19"/>
-      <c r="YJ28" s="19"/>
-      <c r="YK28" s="19"/>
-      <c r="YL28" s="19"/>
-      <c r="YM28" s="19"/>
-      <c r="YN28" s="19"/>
-      <c r="YO28" s="19"/>
-      <c r="YP28" s="19"/>
-      <c r="YQ28" s="19"/>
-      <c r="YR28" s="19"/>
-      <c r="YS28" s="19"/>
-      <c r="YT28" s="19"/>
-      <c r="YU28" s="19"/>
-      <c r="YV28" s="19"/>
-      <c r="YW28" s="19"/>
-      <c r="YX28" s="19"/>
-      <c r="YY28" s="19"/>
-      <c r="YZ28" s="19"/>
-      <c r="ZA28" s="19"/>
-      <c r="ZB28" s="19"/>
-      <c r="ZC28" s="19"/>
-      <c r="ZD28" s="19"/>
-      <c r="ZE28" s="19"/>
-      <c r="ZF28" s="19"/>
-      <c r="ZG28" s="19"/>
-      <c r="ZH28" s="19"/>
-      <c r="ZI28" s="19"/>
-      <c r="ZJ28" s="19"/>
-      <c r="ZK28" s="19"/>
-      <c r="ZL28" s="19"/>
-      <c r="ZM28" s="19"/>
-      <c r="ZN28" s="19"/>
-      <c r="ZO28" s="19"/>
-      <c r="ZP28" s="19"/>
-      <c r="ZQ28" s="19"/>
-      <c r="ZR28" s="19"/>
-      <c r="ZS28" s="19"/>
-      <c r="ZT28" s="19"/>
-      <c r="ZU28" s="19"/>
-      <c r="ZV28" s="19"/>
-      <c r="ZW28" s="19"/>
-      <c r="ZX28" s="19"/>
-      <c r="ZY28" s="19"/>
-      <c r="ZZ28" s="19"/>
-      <c r="AAA28" s="19"/>
-      <c r="AAB28" s="19"/>
-      <c r="AAC28" s="19"/>
-      <c r="AAD28" s="19"/>
-      <c r="AAE28" s="19"/>
-      <c r="AAF28" s="19"/>
-      <c r="AAG28" s="19"/>
-      <c r="AAH28" s="19"/>
-      <c r="AAI28" s="19"/>
-      <c r="AAJ28" s="19"/>
-      <c r="AAK28" s="19"/>
-      <c r="AAL28" s="19"/>
-      <c r="AAM28" s="19"/>
-      <c r="AAN28" s="19"/>
-      <c r="AAO28" s="19"/>
-      <c r="AAP28" s="19"/>
-      <c r="AAQ28" s="19"/>
-      <c r="AAR28" s="19"/>
-      <c r="AAS28" s="19"/>
-      <c r="AAT28" s="19"/>
-      <c r="AAU28" s="19"/>
-      <c r="AAV28" s="19"/>
-      <c r="AAW28" s="19"/>
-      <c r="AAX28" s="19"/>
-      <c r="AAY28" s="19"/>
-      <c r="AAZ28" s="19"/>
-      <c r="ABA28" s="19"/>
-      <c r="ABB28" s="19"/>
-      <c r="ABC28" s="19"/>
-      <c r="ABD28" s="19"/>
-      <c r="ABE28" s="19"/>
-      <c r="ABF28" s="19"/>
-      <c r="ABG28" s="19"/>
-      <c r="ABH28" s="19"/>
-      <c r="ABI28" s="19"/>
-      <c r="ABJ28" s="19"/>
-      <c r="ABK28" s="19"/>
-      <c r="ABL28" s="19"/>
-      <c r="ABM28" s="19"/>
-      <c r="ABN28" s="19"/>
-      <c r="ABO28" s="19"/>
-      <c r="ABP28" s="19"/>
-      <c r="ABQ28" s="19"/>
-      <c r="ABR28" s="19"/>
-      <c r="ABS28" s="19"/>
-      <c r="ABT28" s="19"/>
-      <c r="ABU28" s="19"/>
-      <c r="ABV28" s="19"/>
-      <c r="ABW28" s="19"/>
-      <c r="ABX28" s="19"/>
-      <c r="ABY28" s="19"/>
-      <c r="ABZ28" s="19"/>
-      <c r="ACA28" s="19"/>
-      <c r="ACB28" s="19"/>
-      <c r="ACC28" s="19"/>
-      <c r="ACD28" s="19"/>
-      <c r="ACE28" s="19"/>
-      <c r="ACF28" s="19"/>
-      <c r="ACG28" s="19"/>
-      <c r="ACH28" s="19"/>
-      <c r="ACI28" s="19"/>
-      <c r="ACJ28" s="19"/>
-      <c r="ACK28" s="19"/>
-      <c r="ACL28" s="19"/>
-      <c r="ACM28" s="19"/>
-      <c r="ACN28" s="19"/>
-      <c r="ACO28" s="19"/>
-      <c r="ACP28" s="19"/>
-      <c r="ACQ28" s="19"/>
-      <c r="ACR28" s="19"/>
-      <c r="ACS28" s="19"/>
-      <c r="ACT28" s="19"/>
-      <c r="ACU28" s="19"/>
-      <c r="ACV28" s="19"/>
-      <c r="ACW28" s="19"/>
-      <c r="ACX28" s="19"/>
-      <c r="ACY28" s="19"/>
-      <c r="ACZ28" s="19"/>
-      <c r="ADA28" s="19"/>
-      <c r="ADB28" s="19"/>
-      <c r="ADC28" s="19"/>
-      <c r="ADD28" s="19"/>
-      <c r="ADE28" s="19"/>
-      <c r="ADF28" s="19"/>
-      <c r="ADG28" s="19"/>
-      <c r="ADH28" s="19"/>
-      <c r="ADI28" s="19"/>
-      <c r="ADJ28" s="19"/>
-      <c r="ADK28" s="19"/>
-      <c r="ADL28" s="19"/>
-      <c r="ADM28" s="19"/>
-      <c r="ADN28" s="19"/>
-      <c r="ADO28" s="19"/>
-      <c r="ADP28" s="19"/>
-      <c r="ADQ28" s="19"/>
-      <c r="ADR28" s="19"/>
-      <c r="ADS28" s="19"/>
-      <c r="ADT28" s="19"/>
-      <c r="ADU28" s="19"/>
-      <c r="ADV28" s="19"/>
-      <c r="ADW28" s="19"/>
-      <c r="ADX28" s="19"/>
-      <c r="ADY28" s="19"/>
-      <c r="ADZ28" s="19"/>
-      <c r="AEA28" s="19"/>
-      <c r="AEB28" s="19"/>
-      <c r="AEC28" s="19"/>
-      <c r="AED28" s="19"/>
-      <c r="AEE28" s="19"/>
-      <c r="AEF28" s="19"/>
-      <c r="AEG28" s="19"/>
-      <c r="AEH28" s="19"/>
-      <c r="AEI28" s="19"/>
-      <c r="AEJ28" s="19"/>
-      <c r="AEK28" s="19"/>
-      <c r="AEL28" s="19"/>
-      <c r="AEM28" s="19"/>
-      <c r="AEN28" s="19"/>
-      <c r="AEO28" s="19"/>
-      <c r="AEP28" s="19"/>
-      <c r="AEQ28" s="19"/>
-      <c r="AER28" s="19"/>
-      <c r="AES28" s="19"/>
-      <c r="AET28" s="19"/>
-      <c r="AEU28" s="19"/>
-      <c r="AEV28" s="19"/>
-      <c r="AEW28" s="19"/>
-      <c r="AEX28" s="19"/>
-      <c r="AEY28" s="19"/>
-      <c r="AEZ28" s="19"/>
-      <c r="AFA28" s="19"/>
-      <c r="AFB28" s="19"/>
-      <c r="AFC28" s="19"/>
-      <c r="AFD28" s="19"/>
-      <c r="AFE28" s="19"/>
-      <c r="AFF28" s="19"/>
-      <c r="AFG28" s="19"/>
-      <c r="AFH28" s="19"/>
-      <c r="AFI28" s="19"/>
-      <c r="AFJ28" s="19"/>
-      <c r="AFK28" s="19"/>
-      <c r="AFL28" s="19"/>
-      <c r="AFM28" s="19"/>
-      <c r="AFN28" s="19"/>
-      <c r="AFO28" s="19"/>
-      <c r="AFP28" s="19"/>
-      <c r="AFQ28" s="19"/>
-      <c r="AFR28" s="19"/>
-      <c r="AFS28" s="19"/>
-      <c r="AFT28" s="19"/>
-      <c r="AFU28" s="19"/>
-      <c r="AFV28" s="19"/>
-      <c r="AFW28" s="19"/>
-      <c r="AFX28" s="19"/>
-      <c r="AFY28" s="19"/>
-      <c r="AFZ28" s="19"/>
-      <c r="AGA28" s="19"/>
-      <c r="AGB28" s="19"/>
-      <c r="AGC28" s="19"/>
-      <c r="AGD28" s="19"/>
-      <c r="AGE28" s="19"/>
-      <c r="AGF28" s="19"/>
-      <c r="AGG28" s="19"/>
-      <c r="AGH28" s="19"/>
-      <c r="AGI28" s="19"/>
-      <c r="AGJ28" s="19"/>
-      <c r="AGK28" s="19"/>
-      <c r="AGL28" s="19"/>
-      <c r="AGM28" s="19"/>
-      <c r="AGN28" s="19"/>
-      <c r="AGO28" s="19"/>
-      <c r="AGP28" s="19"/>
-      <c r="AGQ28" s="19"/>
-      <c r="AGR28" s="19"/>
-      <c r="AGS28" s="19"/>
-      <c r="AGT28" s="19"/>
-      <c r="AGU28" s="19"/>
-      <c r="AGV28" s="19"/>
-      <c r="AGW28" s="19"/>
-      <c r="AGX28" s="19"/>
-      <c r="AGY28" s="19"/>
-      <c r="AGZ28" s="19"/>
-      <c r="AHA28" s="19"/>
-      <c r="AHB28" s="19"/>
-      <c r="AHC28" s="19"/>
-      <c r="AHD28" s="19"/>
-      <c r="AHE28" s="19"/>
-      <c r="AHF28" s="19"/>
-      <c r="AHG28" s="19"/>
-      <c r="AHH28" s="19"/>
-      <c r="AHI28" s="19"/>
-      <c r="AHJ28" s="19"/>
-      <c r="AHK28" s="19"/>
-      <c r="AHL28" s="19"/>
-      <c r="AHM28" s="19"/>
-      <c r="AHN28" s="19"/>
-      <c r="AHO28" s="19"/>
-      <c r="AHP28" s="19"/>
-      <c r="AHQ28" s="19"/>
-      <c r="AHR28" s="19"/>
-      <c r="AHS28" s="19"/>
-      <c r="AHT28" s="19"/>
-      <c r="AHU28" s="19"/>
-      <c r="AHV28" s="19"/>
-      <c r="AHW28" s="19"/>
-      <c r="AHX28" s="19"/>
-      <c r="AHY28" s="19"/>
-      <c r="AHZ28" s="19"/>
-      <c r="AIA28" s="19"/>
-      <c r="AIB28" s="19"/>
-      <c r="AIC28" s="19"/>
-      <c r="AID28" s="19"/>
-      <c r="AIE28" s="19"/>
-      <c r="AIF28" s="19"/>
-      <c r="AIG28" s="19"/>
-      <c r="AIH28" s="19"/>
-      <c r="AII28" s="19"/>
-      <c r="AIJ28" s="19"/>
-      <c r="AIK28" s="19"/>
-      <c r="AIL28" s="19"/>
-      <c r="AIM28" s="19"/>
-      <c r="AIN28" s="19"/>
-      <c r="AIO28" s="19"/>
-      <c r="AIP28" s="19"/>
-      <c r="AIQ28" s="19"/>
-      <c r="AIR28" s="19"/>
-      <c r="AIS28" s="19"/>
-      <c r="AIT28" s="19"/>
-      <c r="AIU28" s="19"/>
-      <c r="AIV28" s="19"/>
-      <c r="AIW28" s="19"/>
-      <c r="AIX28" s="19"/>
-      <c r="AIY28" s="19"/>
-      <c r="AIZ28" s="19"/>
-      <c r="AJA28" s="19"/>
-      <c r="AJB28" s="19"/>
-      <c r="AJC28" s="19"/>
-      <c r="AJD28" s="19"/>
-      <c r="AJE28" s="19"/>
-      <c r="AJF28" s="19"/>
-      <c r="AJG28" s="19"/>
-      <c r="AJH28" s="19"/>
-      <c r="AJI28" s="19"/>
-      <c r="AJJ28" s="19"/>
-      <c r="AJK28" s="19"/>
-      <c r="AJL28" s="19"/>
-      <c r="AJM28" s="19"/>
-      <c r="AJN28" s="19"/>
-      <c r="AJO28" s="19"/>
-      <c r="AJP28" s="19"/>
-      <c r="AJQ28" s="19"/>
-      <c r="AJR28" s="19"/>
-      <c r="AJS28" s="19"/>
-      <c r="AJT28" s="19"/>
-      <c r="AJU28" s="19"/>
-      <c r="AJV28" s="19"/>
-      <c r="AJW28" s="19"/>
-      <c r="AJX28" s="19"/>
-      <c r="AJY28" s="19"/>
-      <c r="AJZ28" s="19"/>
-      <c r="AKA28" s="19"/>
-      <c r="AKB28" s="19"/>
-      <c r="AKC28" s="19"/>
-      <c r="AKD28" s="19"/>
-      <c r="AKE28" s="19"/>
-      <c r="AKF28" s="19"/>
-      <c r="AKG28" s="19"/>
-      <c r="AKH28" s="19"/>
-      <c r="AKI28" s="19"/>
-      <c r="AKJ28" s="19"/>
-      <c r="AKK28" s="19"/>
-      <c r="AKL28" s="19"/>
-      <c r="AKM28" s="19"/>
-      <c r="AKN28" s="19"/>
-      <c r="AKO28" s="19"/>
-      <c r="AKP28" s="19"/>
-      <c r="AKQ28" s="19"/>
-      <c r="AKR28" s="19"/>
-      <c r="AKS28" s="19"/>
-      <c r="AKT28" s="19"/>
-      <c r="AKU28" s="19"/>
-      <c r="AKV28" s="19"/>
-      <c r="AKW28" s="19"/>
-      <c r="AKX28" s="19"/>
-      <c r="AKY28" s="19"/>
-      <c r="AKZ28" s="19"/>
-      <c r="ALA28" s="19"/>
-      <c r="ALB28" s="19"/>
-      <c r="ALC28" s="19"/>
-      <c r="ALD28" s="19"/>
-      <c r="ALE28" s="19"/>
-      <c r="ALF28" s="19"/>
-      <c r="ALG28" s="19"/>
-      <c r="ALH28" s="19"/>
-      <c r="ALI28" s="19"/>
-      <c r="ALJ28" s="19"/>
-      <c r="ALK28" s="19"/>
-      <c r="ALL28" s="19"/>
-      <c r="ALM28" s="19"/>
-      <c r="ALN28" s="19"/>
-      <c r="ALO28" s="19"/>
-      <c r="ALP28" s="19"/>
-      <c r="ALQ28" s="19"/>
-      <c r="ALR28" s="19"/>
-      <c r="ALS28" s="19"/>
-      <c r="ALT28" s="19"/>
-      <c r="ALU28" s="19"/>
-      <c r="ALV28" s="19"/>
-      <c r="ALW28" s="19"/>
-      <c r="ALX28" s="19"/>
-      <c r="ALY28" s="19"/>
-      <c r="ALZ28" s="19"/>
-      <c r="AMA28" s="19"/>
-      <c r="AMB28" s="19"/>
-      <c r="AMC28" s="19"/>
-      <c r="AMD28" s="19"/>
-      <c r="AME28" s="19"/>
-      <c r="AMF28" s="19"/>
-      <c r="AMG28" s="19"/>
-      <c r="AMH28" s="19"/>
-      <c r="AMI28" s="19"/>
-      <c r="AMJ28" s="19"/>
-      <c r="AMK28" s="19"/>
-      <c r="AML28" s="19"/>
-      <c r="AMM28" s="19"/>
-      <c r="AMN28" s="19"/>
-      <c r="AMO28" s="19"/>
-      <c r="AMP28" s="19"/>
-      <c r="AMQ28" s="19"/>
-      <c r="AMR28" s="19"/>
     </row>
     <row r="29" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A29" s="48" t="s">
-        <v>16</v>
+      <c r="A29" s="41" t="s">
+        <v>17</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="44"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
       <c r="AA29" s="19"/>
-      <c r="AB29" s="15"/>
+      <c r="AB29" s="19"/>
       <c r="AC29" s="19"/>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
@@ -11831,8 +10853,10 @@
       <c r="AMR29" s="19"/>
     </row>
     <row r="30" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="41"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -11852,17 +10876,17 @@
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
       <c r="U30" s="14"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="45"/>
-      <c r="X30" s="19"/>
-      <c r="Y30" s="44"/>
-      <c r="Z30" s="15"/>
-      <c r="AA30" s="15"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="19"/>
       <c r="AB30" s="15"/>
-      <c r="AC30" s="15"/>
-      <c r="AD30" s="15"/>
-      <c r="AE30" s="15"/>
-      <c r="AF30" s="15"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
+      <c r="AE30" s="19"/>
+      <c r="AF30" s="19"/>
       <c r="AG30" s="15"/>
       <c r="AH30" s="15"/>
       <c r="AI30" s="15"/>
@@ -12867,29 +11891,29 @@
     <row r="31" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="19"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="42"/>
       <c r="X31" s="19"/>
-      <c r="Y31" s="19"/>
+      <c r="Y31" s="41"/>
       <c r="Z31" s="15"/>
       <c r="AA31" s="15"/>
       <c r="AB31" s="15"/>
@@ -13899,8 +12923,8 @@
       <c r="AMR31" s="19"/>
     </row>
     <row r="32" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A32" s="46"/>
-      <c r="B32" s="19"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
@@ -14932,62 +13956,1042 @@
       <c r="AMQ32" s="19"/>
       <c r="AMR32" s="19"/>
     </row>
-    <row r="33" spans="2:77" x14ac:dyDescent="0.3">
-      <c r="B33" s="11"/>
-      <c r="Z33" s="3"/>
-      <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
-      <c r="AF33" s="3"/>
-      <c r="AG33" s="3"/>
-      <c r="AH33" s="3"/>
-      <c r="AI33" s="3"/>
-      <c r="AJ33" s="3"/>
-      <c r="AK33" s="3"/>
-      <c r="AL33" s="3"/>
-      <c r="AM33" s="3"/>
-      <c r="AN33" s="3"/>
-      <c r="AO33" s="3"/>
-      <c r="AP33" s="3"/>
-      <c r="AQ33" s="3"/>
-      <c r="AR33" s="3"/>
-      <c r="AS33" s="3"/>
-      <c r="AT33" s="3"/>
-      <c r="AU33" s="3"/>
-      <c r="AV33" s="3"/>
-      <c r="AW33" s="3"/>
-      <c r="AX33" s="3"/>
-      <c r="AY33" s="3"/>
-      <c r="AZ33" s="3"/>
-      <c r="BA33" s="3"/>
-      <c r="BB33" s="3"/>
-      <c r="BC33" s="3"/>
-      <c r="BD33" s="3"/>
-      <c r="BE33" s="3"/>
-      <c r="BF33" s="3"/>
-      <c r="BG33" s="3"/>
-      <c r="BH33" s="3"/>
-      <c r="BI33" s="3"/>
-      <c r="BJ33" s="3"/>
-      <c r="BK33" s="3"/>
-      <c r="BL33" s="3"/>
-      <c r="BM33" s="3"/>
-      <c r="BN33" s="3"/>
-      <c r="BO33" s="3"/>
-      <c r="BP33" s="3"/>
-      <c r="BQ33" s="3"/>
-      <c r="BR33" s="3"/>
-      <c r="BS33" s="3"/>
-      <c r="BT33" s="3"/>
-      <c r="BU33" s="3"/>
-      <c r="BV33" s="3"/>
-      <c r="BW33" s="3"/>
-      <c r="BX33" s="3"/>
-      <c r="BY33" s="3"/>
-    </row>
-    <row r="34" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A33" s="43"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
+      <c r="AD33" s="15"/>
+      <c r="AE33" s="15"/>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="15"/>
+      <c r="AH33" s="15"/>
+      <c r="AI33" s="15"/>
+      <c r="AJ33" s="15"/>
+      <c r="AK33" s="15"/>
+      <c r="AL33" s="15"/>
+      <c r="AM33" s="15"/>
+      <c r="AN33" s="15"/>
+      <c r="AO33" s="15"/>
+      <c r="AP33" s="15"/>
+      <c r="AQ33" s="15"/>
+      <c r="AR33" s="15"/>
+      <c r="AS33" s="15"/>
+      <c r="AT33" s="15"/>
+      <c r="AU33" s="15"/>
+      <c r="AV33" s="15"/>
+      <c r="AW33" s="15"/>
+      <c r="AX33" s="15"/>
+      <c r="AY33" s="15"/>
+      <c r="AZ33" s="15"/>
+      <c r="BA33" s="15"/>
+      <c r="BB33" s="15"/>
+      <c r="BC33" s="15"/>
+      <c r="BD33" s="15"/>
+      <c r="BE33" s="15"/>
+      <c r="BF33" s="15"/>
+      <c r="BG33" s="15"/>
+      <c r="BH33" s="15"/>
+      <c r="BI33" s="15"/>
+      <c r="BJ33" s="15"/>
+      <c r="BK33" s="15"/>
+      <c r="BL33" s="15"/>
+      <c r="BM33" s="15"/>
+      <c r="BN33" s="15"/>
+      <c r="BO33" s="15"/>
+      <c r="BP33" s="15"/>
+      <c r="BQ33" s="15"/>
+      <c r="BR33" s="15"/>
+      <c r="BS33" s="15"/>
+      <c r="BT33" s="15"/>
+      <c r="BU33" s="15"/>
+      <c r="BV33" s="15"/>
+      <c r="BW33" s="15"/>
+      <c r="BX33" s="15"/>
+      <c r="BY33" s="15"/>
+      <c r="BZ33" s="19"/>
+      <c r="CA33" s="19"/>
+      <c r="CB33" s="19"/>
+      <c r="CC33" s="19"/>
+      <c r="CD33" s="19"/>
+      <c r="CE33" s="19"/>
+      <c r="CF33" s="19"/>
+      <c r="CG33" s="19"/>
+      <c r="CH33" s="19"/>
+      <c r="CI33" s="19"/>
+      <c r="CJ33" s="19"/>
+      <c r="CK33" s="19"/>
+      <c r="CL33" s="19"/>
+      <c r="CM33" s="19"/>
+      <c r="CN33" s="19"/>
+      <c r="CO33" s="19"/>
+      <c r="CP33" s="19"/>
+      <c r="CQ33" s="19"/>
+      <c r="CR33" s="19"/>
+      <c r="CS33" s="19"/>
+      <c r="CT33" s="19"/>
+      <c r="CU33" s="19"/>
+      <c r="CV33" s="19"/>
+      <c r="CW33" s="19"/>
+      <c r="CX33" s="19"/>
+      <c r="CY33" s="19"/>
+      <c r="CZ33" s="19"/>
+      <c r="DA33" s="19"/>
+      <c r="DB33" s="19"/>
+      <c r="DC33" s="19"/>
+      <c r="DD33" s="19"/>
+      <c r="DE33" s="19"/>
+      <c r="DF33" s="19"/>
+      <c r="DG33" s="19"/>
+      <c r="DH33" s="19"/>
+      <c r="DI33" s="19"/>
+      <c r="DJ33" s="19"/>
+      <c r="DK33" s="19"/>
+      <c r="DL33" s="19"/>
+      <c r="DM33" s="19"/>
+      <c r="DN33" s="19"/>
+      <c r="DO33" s="19"/>
+      <c r="DP33" s="19"/>
+      <c r="DQ33" s="19"/>
+      <c r="DR33" s="19"/>
+      <c r="DS33" s="19"/>
+      <c r="DT33" s="19"/>
+      <c r="DU33" s="19"/>
+      <c r="DV33" s="19"/>
+      <c r="DW33" s="19"/>
+      <c r="DX33" s="19"/>
+      <c r="DY33" s="19"/>
+      <c r="DZ33" s="19"/>
+      <c r="EA33" s="19"/>
+      <c r="EB33" s="19"/>
+      <c r="EC33" s="19"/>
+      <c r="ED33" s="19"/>
+      <c r="EE33" s="19"/>
+      <c r="EF33" s="19"/>
+      <c r="EG33" s="19"/>
+      <c r="EH33" s="19"/>
+      <c r="EI33" s="19"/>
+      <c r="EJ33" s="19"/>
+      <c r="EK33" s="19"/>
+      <c r="EL33" s="19"/>
+      <c r="EM33" s="19"/>
+      <c r="EN33" s="19"/>
+      <c r="EO33" s="19"/>
+      <c r="EP33" s="19"/>
+      <c r="EQ33" s="19"/>
+      <c r="ER33" s="19"/>
+      <c r="ES33" s="19"/>
+      <c r="ET33" s="19"/>
+      <c r="EU33" s="19"/>
+      <c r="EV33" s="19"/>
+      <c r="EW33" s="19"/>
+      <c r="EX33" s="19"/>
+      <c r="EY33" s="19"/>
+      <c r="EZ33" s="19"/>
+      <c r="FA33" s="19"/>
+      <c r="FB33" s="19"/>
+      <c r="FC33" s="19"/>
+      <c r="FD33" s="19"/>
+      <c r="FE33" s="19"/>
+      <c r="FF33" s="19"/>
+      <c r="FG33" s="19"/>
+      <c r="FH33" s="19"/>
+      <c r="FI33" s="19"/>
+      <c r="FJ33" s="19"/>
+      <c r="FK33" s="19"/>
+      <c r="FL33" s="19"/>
+      <c r="FM33" s="19"/>
+      <c r="FN33" s="19"/>
+      <c r="FO33" s="19"/>
+      <c r="FP33" s="19"/>
+      <c r="FQ33" s="19"/>
+      <c r="FR33" s="19"/>
+      <c r="FS33" s="19"/>
+      <c r="FT33" s="19"/>
+      <c r="FU33" s="19"/>
+      <c r="FV33" s="19"/>
+      <c r="FW33" s="19"/>
+      <c r="FX33" s="19"/>
+      <c r="FY33" s="19"/>
+      <c r="FZ33" s="19"/>
+      <c r="GA33" s="19"/>
+      <c r="GB33" s="19"/>
+      <c r="GC33" s="19"/>
+      <c r="GD33" s="19"/>
+      <c r="GE33" s="19"/>
+      <c r="GF33" s="19"/>
+      <c r="GG33" s="19"/>
+      <c r="GH33" s="19"/>
+      <c r="GI33" s="19"/>
+      <c r="GJ33" s="19"/>
+      <c r="GK33" s="19"/>
+      <c r="GL33" s="19"/>
+      <c r="GM33" s="19"/>
+      <c r="GN33" s="19"/>
+      <c r="GO33" s="19"/>
+      <c r="GP33" s="19"/>
+      <c r="GQ33" s="19"/>
+      <c r="GR33" s="19"/>
+      <c r="GS33" s="19"/>
+      <c r="GT33" s="19"/>
+      <c r="GU33" s="19"/>
+      <c r="GV33" s="19"/>
+      <c r="GW33" s="19"/>
+      <c r="GX33" s="19"/>
+      <c r="GY33" s="19"/>
+      <c r="GZ33" s="19"/>
+      <c r="HA33" s="19"/>
+      <c r="HB33" s="19"/>
+      <c r="HC33" s="19"/>
+      <c r="HD33" s="19"/>
+      <c r="HE33" s="19"/>
+      <c r="HF33" s="19"/>
+      <c r="HG33" s="19"/>
+      <c r="HH33" s="19"/>
+      <c r="HI33" s="19"/>
+      <c r="HJ33" s="19"/>
+      <c r="HK33" s="19"/>
+      <c r="HL33" s="19"/>
+      <c r="HM33" s="19"/>
+      <c r="HN33" s="19"/>
+      <c r="HO33" s="19"/>
+      <c r="HP33" s="19"/>
+      <c r="HQ33" s="19"/>
+      <c r="HR33" s="19"/>
+      <c r="HS33" s="19"/>
+      <c r="HT33" s="19"/>
+      <c r="HU33" s="19"/>
+      <c r="HV33" s="19"/>
+      <c r="HW33" s="19"/>
+      <c r="HX33" s="19"/>
+      <c r="HY33" s="19"/>
+      <c r="HZ33" s="19"/>
+      <c r="IA33" s="19"/>
+      <c r="IB33" s="19"/>
+      <c r="IC33" s="19"/>
+      <c r="ID33" s="19"/>
+      <c r="IE33" s="19"/>
+      <c r="IF33" s="19"/>
+      <c r="IG33" s="19"/>
+      <c r="IH33" s="19"/>
+      <c r="II33" s="19"/>
+      <c r="IJ33" s="19"/>
+      <c r="IK33" s="19"/>
+      <c r="IL33" s="19"/>
+      <c r="IM33" s="19"/>
+      <c r="IN33" s="19"/>
+      <c r="IO33" s="19"/>
+      <c r="IP33" s="19"/>
+      <c r="IQ33" s="19"/>
+      <c r="IR33" s="19"/>
+      <c r="IS33" s="19"/>
+      <c r="IT33" s="19"/>
+      <c r="IU33" s="19"/>
+      <c r="IV33" s="19"/>
+      <c r="IW33" s="19"/>
+      <c r="IX33" s="19"/>
+      <c r="IY33" s="19"/>
+      <c r="IZ33" s="19"/>
+      <c r="JA33" s="19"/>
+      <c r="JB33" s="19"/>
+      <c r="JC33" s="19"/>
+      <c r="JD33" s="19"/>
+      <c r="JE33" s="19"/>
+      <c r="JF33" s="19"/>
+      <c r="JG33" s="19"/>
+      <c r="JH33" s="19"/>
+      <c r="JI33" s="19"/>
+      <c r="JJ33" s="19"/>
+      <c r="JK33" s="19"/>
+      <c r="JL33" s="19"/>
+      <c r="JM33" s="19"/>
+      <c r="JN33" s="19"/>
+      <c r="JO33" s="19"/>
+      <c r="JP33" s="19"/>
+      <c r="JQ33" s="19"/>
+      <c r="JR33" s="19"/>
+      <c r="JS33" s="19"/>
+      <c r="JT33" s="19"/>
+      <c r="JU33" s="19"/>
+      <c r="JV33" s="19"/>
+      <c r="JW33" s="19"/>
+      <c r="JX33" s="19"/>
+      <c r="JY33" s="19"/>
+      <c r="JZ33" s="19"/>
+      <c r="KA33" s="19"/>
+      <c r="KB33" s="19"/>
+      <c r="KC33" s="19"/>
+      <c r="KD33" s="19"/>
+      <c r="KE33" s="19"/>
+      <c r="KF33" s="19"/>
+      <c r="KG33" s="19"/>
+      <c r="KH33" s="19"/>
+      <c r="KI33" s="19"/>
+      <c r="KJ33" s="19"/>
+      <c r="KK33" s="19"/>
+      <c r="KL33" s="19"/>
+      <c r="KM33" s="19"/>
+      <c r="KN33" s="19"/>
+      <c r="KO33" s="19"/>
+      <c r="KP33" s="19"/>
+      <c r="KQ33" s="19"/>
+      <c r="KR33" s="19"/>
+      <c r="KS33" s="19"/>
+      <c r="KT33" s="19"/>
+      <c r="KU33" s="19"/>
+      <c r="KV33" s="19"/>
+      <c r="KW33" s="19"/>
+      <c r="KX33" s="19"/>
+      <c r="KY33" s="19"/>
+      <c r="KZ33" s="19"/>
+      <c r="LA33" s="19"/>
+      <c r="LB33" s="19"/>
+      <c r="LC33" s="19"/>
+      <c r="LD33" s="19"/>
+      <c r="LE33" s="19"/>
+      <c r="LF33" s="19"/>
+      <c r="LG33" s="19"/>
+      <c r="LH33" s="19"/>
+      <c r="LI33" s="19"/>
+      <c r="LJ33" s="19"/>
+      <c r="LK33" s="19"/>
+      <c r="LL33" s="19"/>
+      <c r="LM33" s="19"/>
+      <c r="LN33" s="19"/>
+      <c r="LO33" s="19"/>
+      <c r="LP33" s="19"/>
+      <c r="LQ33" s="19"/>
+      <c r="LR33" s="19"/>
+      <c r="LS33" s="19"/>
+      <c r="LT33" s="19"/>
+      <c r="LU33" s="19"/>
+      <c r="LV33" s="19"/>
+      <c r="LW33" s="19"/>
+      <c r="LX33" s="19"/>
+      <c r="LY33" s="19"/>
+      <c r="LZ33" s="19"/>
+      <c r="MA33" s="19"/>
+      <c r="MB33" s="19"/>
+      <c r="MC33" s="19"/>
+      <c r="MD33" s="19"/>
+      <c r="ME33" s="19"/>
+      <c r="MF33" s="19"/>
+      <c r="MG33" s="19"/>
+      <c r="MH33" s="19"/>
+      <c r="MI33" s="19"/>
+      <c r="MJ33" s="19"/>
+      <c r="MK33" s="19"/>
+      <c r="ML33" s="19"/>
+      <c r="MM33" s="19"/>
+      <c r="MN33" s="19"/>
+      <c r="MO33" s="19"/>
+      <c r="MP33" s="19"/>
+      <c r="MQ33" s="19"/>
+      <c r="MR33" s="19"/>
+      <c r="MS33" s="19"/>
+      <c r="MT33" s="19"/>
+      <c r="MU33" s="19"/>
+      <c r="MV33" s="19"/>
+      <c r="MW33" s="19"/>
+      <c r="MX33" s="19"/>
+      <c r="MY33" s="19"/>
+      <c r="MZ33" s="19"/>
+      <c r="NA33" s="19"/>
+      <c r="NB33" s="19"/>
+      <c r="NC33" s="19"/>
+      <c r="ND33" s="19"/>
+      <c r="NE33" s="19"/>
+      <c r="NF33" s="19"/>
+      <c r="NG33" s="19"/>
+      <c r="NH33" s="19"/>
+      <c r="NI33" s="19"/>
+      <c r="NJ33" s="19"/>
+      <c r="NK33" s="19"/>
+      <c r="NL33" s="19"/>
+      <c r="NM33" s="19"/>
+      <c r="NN33" s="19"/>
+      <c r="NO33" s="19"/>
+      <c r="NP33" s="19"/>
+      <c r="NQ33" s="19"/>
+      <c r="NR33" s="19"/>
+      <c r="NS33" s="19"/>
+      <c r="NT33" s="19"/>
+      <c r="NU33" s="19"/>
+      <c r="NV33" s="19"/>
+      <c r="NW33" s="19"/>
+      <c r="NX33" s="19"/>
+      <c r="NY33" s="19"/>
+      <c r="NZ33" s="19"/>
+      <c r="OA33" s="19"/>
+      <c r="OB33" s="19"/>
+      <c r="OC33" s="19"/>
+      <c r="OD33" s="19"/>
+      <c r="OE33" s="19"/>
+      <c r="OF33" s="19"/>
+      <c r="OG33" s="19"/>
+      <c r="OH33" s="19"/>
+      <c r="OI33" s="19"/>
+      <c r="OJ33" s="19"/>
+      <c r="OK33" s="19"/>
+      <c r="OL33" s="19"/>
+      <c r="OM33" s="19"/>
+      <c r="ON33" s="19"/>
+      <c r="OO33" s="19"/>
+      <c r="OP33" s="19"/>
+      <c r="OQ33" s="19"/>
+      <c r="OR33" s="19"/>
+      <c r="OS33" s="19"/>
+      <c r="OT33" s="19"/>
+      <c r="OU33" s="19"/>
+      <c r="OV33" s="19"/>
+      <c r="OW33" s="19"/>
+      <c r="OX33" s="19"/>
+      <c r="OY33" s="19"/>
+      <c r="OZ33" s="19"/>
+      <c r="PA33" s="19"/>
+      <c r="PB33" s="19"/>
+      <c r="PC33" s="19"/>
+      <c r="PD33" s="19"/>
+      <c r="PE33" s="19"/>
+      <c r="PF33" s="19"/>
+      <c r="PG33" s="19"/>
+      <c r="PH33" s="19"/>
+      <c r="PI33" s="19"/>
+      <c r="PJ33" s="19"/>
+      <c r="PK33" s="19"/>
+      <c r="PL33" s="19"/>
+      <c r="PM33" s="19"/>
+      <c r="PN33" s="19"/>
+      <c r="PO33" s="19"/>
+      <c r="PP33" s="19"/>
+      <c r="PQ33" s="19"/>
+      <c r="PR33" s="19"/>
+      <c r="PS33" s="19"/>
+      <c r="PT33" s="19"/>
+      <c r="PU33" s="19"/>
+      <c r="PV33" s="19"/>
+      <c r="PW33" s="19"/>
+      <c r="PX33" s="19"/>
+      <c r="PY33" s="19"/>
+      <c r="PZ33" s="19"/>
+      <c r="QA33" s="19"/>
+      <c r="QB33" s="19"/>
+      <c r="QC33" s="19"/>
+      <c r="QD33" s="19"/>
+      <c r="QE33" s="19"/>
+      <c r="QF33" s="19"/>
+      <c r="QG33" s="19"/>
+      <c r="QH33" s="19"/>
+      <c r="QI33" s="19"/>
+      <c r="QJ33" s="19"/>
+      <c r="QK33" s="19"/>
+      <c r="QL33" s="19"/>
+      <c r="QM33" s="19"/>
+      <c r="QN33" s="19"/>
+      <c r="QO33" s="19"/>
+      <c r="QP33" s="19"/>
+      <c r="QQ33" s="19"/>
+      <c r="QR33" s="19"/>
+      <c r="QS33" s="19"/>
+      <c r="QT33" s="19"/>
+      <c r="QU33" s="19"/>
+      <c r="QV33" s="19"/>
+      <c r="QW33" s="19"/>
+      <c r="QX33" s="19"/>
+      <c r="QY33" s="19"/>
+      <c r="QZ33" s="19"/>
+      <c r="RA33" s="19"/>
+      <c r="RB33" s="19"/>
+      <c r="RC33" s="19"/>
+      <c r="RD33" s="19"/>
+      <c r="RE33" s="19"/>
+      <c r="RF33" s="19"/>
+      <c r="RG33" s="19"/>
+      <c r="RH33" s="19"/>
+      <c r="RI33" s="19"/>
+      <c r="RJ33" s="19"/>
+      <c r="RK33" s="19"/>
+      <c r="RL33" s="19"/>
+      <c r="RM33" s="19"/>
+      <c r="RN33" s="19"/>
+      <c r="RO33" s="19"/>
+      <c r="RP33" s="19"/>
+      <c r="RQ33" s="19"/>
+      <c r="RR33" s="19"/>
+      <c r="RS33" s="19"/>
+      <c r="RT33" s="19"/>
+      <c r="RU33" s="19"/>
+      <c r="RV33" s="19"/>
+      <c r="RW33" s="19"/>
+      <c r="RX33" s="19"/>
+      <c r="RY33" s="19"/>
+      <c r="RZ33" s="19"/>
+      <c r="SA33" s="19"/>
+      <c r="SB33" s="19"/>
+      <c r="SC33" s="19"/>
+      <c r="SD33" s="19"/>
+      <c r="SE33" s="19"/>
+      <c r="SF33" s="19"/>
+      <c r="SG33" s="19"/>
+      <c r="SH33" s="19"/>
+      <c r="SI33" s="19"/>
+      <c r="SJ33" s="19"/>
+      <c r="SK33" s="19"/>
+      <c r="SL33" s="19"/>
+      <c r="SM33" s="19"/>
+      <c r="SN33" s="19"/>
+      <c r="SO33" s="19"/>
+      <c r="SP33" s="19"/>
+      <c r="SQ33" s="19"/>
+      <c r="SR33" s="19"/>
+      <c r="SS33" s="19"/>
+      <c r="ST33" s="19"/>
+      <c r="SU33" s="19"/>
+      <c r="SV33" s="19"/>
+      <c r="SW33" s="19"/>
+      <c r="SX33" s="19"/>
+      <c r="SY33" s="19"/>
+      <c r="SZ33" s="19"/>
+      <c r="TA33" s="19"/>
+      <c r="TB33" s="19"/>
+      <c r="TC33" s="19"/>
+      <c r="TD33" s="19"/>
+      <c r="TE33" s="19"/>
+      <c r="TF33" s="19"/>
+      <c r="TG33" s="19"/>
+      <c r="TH33" s="19"/>
+      <c r="TI33" s="19"/>
+      <c r="TJ33" s="19"/>
+      <c r="TK33" s="19"/>
+      <c r="TL33" s="19"/>
+      <c r="TM33" s="19"/>
+      <c r="TN33" s="19"/>
+      <c r="TO33" s="19"/>
+      <c r="TP33" s="19"/>
+      <c r="TQ33" s="19"/>
+      <c r="TR33" s="19"/>
+      <c r="TS33" s="19"/>
+      <c r="TT33" s="19"/>
+      <c r="TU33" s="19"/>
+      <c r="TV33" s="19"/>
+      <c r="TW33" s="19"/>
+      <c r="TX33" s="19"/>
+      <c r="TY33" s="19"/>
+      <c r="TZ33" s="19"/>
+      <c r="UA33" s="19"/>
+      <c r="UB33" s="19"/>
+      <c r="UC33" s="19"/>
+      <c r="UD33" s="19"/>
+      <c r="UE33" s="19"/>
+      <c r="UF33" s="19"/>
+      <c r="UG33" s="19"/>
+      <c r="UH33" s="19"/>
+      <c r="UI33" s="19"/>
+      <c r="UJ33" s="19"/>
+      <c r="UK33" s="19"/>
+      <c r="UL33" s="19"/>
+      <c r="UM33" s="19"/>
+      <c r="UN33" s="19"/>
+      <c r="UO33" s="19"/>
+      <c r="UP33" s="19"/>
+      <c r="UQ33" s="19"/>
+      <c r="UR33" s="19"/>
+      <c r="US33" s="19"/>
+      <c r="UT33" s="19"/>
+      <c r="UU33" s="19"/>
+      <c r="UV33" s="19"/>
+      <c r="UW33" s="19"/>
+      <c r="UX33" s="19"/>
+      <c r="UY33" s="19"/>
+      <c r="UZ33" s="19"/>
+      <c r="VA33" s="19"/>
+      <c r="VB33" s="19"/>
+      <c r="VC33" s="19"/>
+      <c r="VD33" s="19"/>
+      <c r="VE33" s="19"/>
+      <c r="VF33" s="19"/>
+      <c r="VG33" s="19"/>
+      <c r="VH33" s="19"/>
+      <c r="VI33" s="19"/>
+      <c r="VJ33" s="19"/>
+      <c r="VK33" s="19"/>
+      <c r="VL33" s="19"/>
+      <c r="VM33" s="19"/>
+      <c r="VN33" s="19"/>
+      <c r="VO33" s="19"/>
+      <c r="VP33" s="19"/>
+      <c r="VQ33" s="19"/>
+      <c r="VR33" s="19"/>
+      <c r="VS33" s="19"/>
+      <c r="VT33" s="19"/>
+      <c r="VU33" s="19"/>
+      <c r="VV33" s="19"/>
+      <c r="VW33" s="19"/>
+      <c r="VX33" s="19"/>
+      <c r="VY33" s="19"/>
+      <c r="VZ33" s="19"/>
+      <c r="WA33" s="19"/>
+      <c r="WB33" s="19"/>
+      <c r="WC33" s="19"/>
+      <c r="WD33" s="19"/>
+      <c r="WE33" s="19"/>
+      <c r="WF33" s="19"/>
+      <c r="WG33" s="19"/>
+      <c r="WH33" s="19"/>
+      <c r="WI33" s="19"/>
+      <c r="WJ33" s="19"/>
+      <c r="WK33" s="19"/>
+      <c r="WL33" s="19"/>
+      <c r="WM33" s="19"/>
+      <c r="WN33" s="19"/>
+      <c r="WO33" s="19"/>
+      <c r="WP33" s="19"/>
+      <c r="WQ33" s="19"/>
+      <c r="WR33" s="19"/>
+      <c r="WS33" s="19"/>
+      <c r="WT33" s="19"/>
+      <c r="WU33" s="19"/>
+      <c r="WV33" s="19"/>
+      <c r="WW33" s="19"/>
+      <c r="WX33" s="19"/>
+      <c r="WY33" s="19"/>
+      <c r="WZ33" s="19"/>
+      <c r="XA33" s="19"/>
+      <c r="XB33" s="19"/>
+      <c r="XC33" s="19"/>
+      <c r="XD33" s="19"/>
+      <c r="XE33" s="19"/>
+      <c r="XF33" s="19"/>
+      <c r="XG33" s="19"/>
+      <c r="XH33" s="19"/>
+      <c r="XI33" s="19"/>
+      <c r="XJ33" s="19"/>
+      <c r="XK33" s="19"/>
+      <c r="XL33" s="19"/>
+      <c r="XM33" s="19"/>
+      <c r="XN33" s="19"/>
+      <c r="XO33" s="19"/>
+      <c r="XP33" s="19"/>
+      <c r="XQ33" s="19"/>
+      <c r="XR33" s="19"/>
+      <c r="XS33" s="19"/>
+      <c r="XT33" s="19"/>
+      <c r="XU33" s="19"/>
+      <c r="XV33" s="19"/>
+      <c r="XW33" s="19"/>
+      <c r="XX33" s="19"/>
+      <c r="XY33" s="19"/>
+      <c r="XZ33" s="19"/>
+      <c r="YA33" s="19"/>
+      <c r="YB33" s="19"/>
+      <c r="YC33" s="19"/>
+      <c r="YD33" s="19"/>
+      <c r="YE33" s="19"/>
+      <c r="YF33" s="19"/>
+      <c r="YG33" s="19"/>
+      <c r="YH33" s="19"/>
+      <c r="YI33" s="19"/>
+      <c r="YJ33" s="19"/>
+      <c r="YK33" s="19"/>
+      <c r="YL33" s="19"/>
+      <c r="YM33" s="19"/>
+      <c r="YN33" s="19"/>
+      <c r="YO33" s="19"/>
+      <c r="YP33" s="19"/>
+      <c r="YQ33" s="19"/>
+      <c r="YR33" s="19"/>
+      <c r="YS33" s="19"/>
+      <c r="YT33" s="19"/>
+      <c r="YU33" s="19"/>
+      <c r="YV33" s="19"/>
+      <c r="YW33" s="19"/>
+      <c r="YX33" s="19"/>
+      <c r="YY33" s="19"/>
+      <c r="YZ33" s="19"/>
+      <c r="ZA33" s="19"/>
+      <c r="ZB33" s="19"/>
+      <c r="ZC33" s="19"/>
+      <c r="ZD33" s="19"/>
+      <c r="ZE33" s="19"/>
+      <c r="ZF33" s="19"/>
+      <c r="ZG33" s="19"/>
+      <c r="ZH33" s="19"/>
+      <c r="ZI33" s="19"/>
+      <c r="ZJ33" s="19"/>
+      <c r="ZK33" s="19"/>
+      <c r="ZL33" s="19"/>
+      <c r="ZM33" s="19"/>
+      <c r="ZN33" s="19"/>
+      <c r="ZO33" s="19"/>
+      <c r="ZP33" s="19"/>
+      <c r="ZQ33" s="19"/>
+      <c r="ZR33" s="19"/>
+      <c r="ZS33" s="19"/>
+      <c r="ZT33" s="19"/>
+      <c r="ZU33" s="19"/>
+      <c r="ZV33" s="19"/>
+      <c r="ZW33" s="19"/>
+      <c r="ZX33" s="19"/>
+      <c r="ZY33" s="19"/>
+      <c r="ZZ33" s="19"/>
+      <c r="AAA33" s="19"/>
+      <c r="AAB33" s="19"/>
+      <c r="AAC33" s="19"/>
+      <c r="AAD33" s="19"/>
+      <c r="AAE33" s="19"/>
+      <c r="AAF33" s="19"/>
+      <c r="AAG33" s="19"/>
+      <c r="AAH33" s="19"/>
+      <c r="AAI33" s="19"/>
+      <c r="AAJ33" s="19"/>
+      <c r="AAK33" s="19"/>
+      <c r="AAL33" s="19"/>
+      <c r="AAM33" s="19"/>
+      <c r="AAN33" s="19"/>
+      <c r="AAO33" s="19"/>
+      <c r="AAP33" s="19"/>
+      <c r="AAQ33" s="19"/>
+      <c r="AAR33" s="19"/>
+      <c r="AAS33" s="19"/>
+      <c r="AAT33" s="19"/>
+      <c r="AAU33" s="19"/>
+      <c r="AAV33" s="19"/>
+      <c r="AAW33" s="19"/>
+      <c r="AAX33" s="19"/>
+      <c r="AAY33" s="19"/>
+      <c r="AAZ33" s="19"/>
+      <c r="ABA33" s="19"/>
+      <c r="ABB33" s="19"/>
+      <c r="ABC33" s="19"/>
+      <c r="ABD33" s="19"/>
+      <c r="ABE33" s="19"/>
+      <c r="ABF33" s="19"/>
+      <c r="ABG33" s="19"/>
+      <c r="ABH33" s="19"/>
+      <c r="ABI33" s="19"/>
+      <c r="ABJ33" s="19"/>
+      <c r="ABK33" s="19"/>
+      <c r="ABL33" s="19"/>
+      <c r="ABM33" s="19"/>
+      <c r="ABN33" s="19"/>
+      <c r="ABO33" s="19"/>
+      <c r="ABP33" s="19"/>
+      <c r="ABQ33" s="19"/>
+      <c r="ABR33" s="19"/>
+      <c r="ABS33" s="19"/>
+      <c r="ABT33" s="19"/>
+      <c r="ABU33" s="19"/>
+      <c r="ABV33" s="19"/>
+      <c r="ABW33" s="19"/>
+      <c r="ABX33" s="19"/>
+      <c r="ABY33" s="19"/>
+      <c r="ABZ33" s="19"/>
+      <c r="ACA33" s="19"/>
+      <c r="ACB33" s="19"/>
+      <c r="ACC33" s="19"/>
+      <c r="ACD33" s="19"/>
+      <c r="ACE33" s="19"/>
+      <c r="ACF33" s="19"/>
+      <c r="ACG33" s="19"/>
+      <c r="ACH33" s="19"/>
+      <c r="ACI33" s="19"/>
+      <c r="ACJ33" s="19"/>
+      <c r="ACK33" s="19"/>
+      <c r="ACL33" s="19"/>
+      <c r="ACM33" s="19"/>
+      <c r="ACN33" s="19"/>
+      <c r="ACO33" s="19"/>
+      <c r="ACP33" s="19"/>
+      <c r="ACQ33" s="19"/>
+      <c r="ACR33" s="19"/>
+      <c r="ACS33" s="19"/>
+      <c r="ACT33" s="19"/>
+      <c r="ACU33" s="19"/>
+      <c r="ACV33" s="19"/>
+      <c r="ACW33" s="19"/>
+      <c r="ACX33" s="19"/>
+      <c r="ACY33" s="19"/>
+      <c r="ACZ33" s="19"/>
+      <c r="ADA33" s="19"/>
+      <c r="ADB33" s="19"/>
+      <c r="ADC33" s="19"/>
+      <c r="ADD33" s="19"/>
+      <c r="ADE33" s="19"/>
+      <c r="ADF33" s="19"/>
+      <c r="ADG33" s="19"/>
+      <c r="ADH33" s="19"/>
+      <c r="ADI33" s="19"/>
+      <c r="ADJ33" s="19"/>
+      <c r="ADK33" s="19"/>
+      <c r="ADL33" s="19"/>
+      <c r="ADM33" s="19"/>
+      <c r="ADN33" s="19"/>
+      <c r="ADO33" s="19"/>
+      <c r="ADP33" s="19"/>
+      <c r="ADQ33" s="19"/>
+      <c r="ADR33" s="19"/>
+      <c r="ADS33" s="19"/>
+      <c r="ADT33" s="19"/>
+      <c r="ADU33" s="19"/>
+      <c r="ADV33" s="19"/>
+      <c r="ADW33" s="19"/>
+      <c r="ADX33" s="19"/>
+      <c r="ADY33" s="19"/>
+      <c r="ADZ33" s="19"/>
+      <c r="AEA33" s="19"/>
+      <c r="AEB33" s="19"/>
+      <c r="AEC33" s="19"/>
+      <c r="AED33" s="19"/>
+      <c r="AEE33" s="19"/>
+      <c r="AEF33" s="19"/>
+      <c r="AEG33" s="19"/>
+      <c r="AEH33" s="19"/>
+      <c r="AEI33" s="19"/>
+      <c r="AEJ33" s="19"/>
+      <c r="AEK33" s="19"/>
+      <c r="AEL33" s="19"/>
+      <c r="AEM33" s="19"/>
+      <c r="AEN33" s="19"/>
+      <c r="AEO33" s="19"/>
+      <c r="AEP33" s="19"/>
+      <c r="AEQ33" s="19"/>
+      <c r="AER33" s="19"/>
+      <c r="AES33" s="19"/>
+      <c r="AET33" s="19"/>
+      <c r="AEU33" s="19"/>
+      <c r="AEV33" s="19"/>
+      <c r="AEW33" s="19"/>
+      <c r="AEX33" s="19"/>
+      <c r="AEY33" s="19"/>
+      <c r="AEZ33" s="19"/>
+      <c r="AFA33" s="19"/>
+      <c r="AFB33" s="19"/>
+      <c r="AFC33" s="19"/>
+      <c r="AFD33" s="19"/>
+      <c r="AFE33" s="19"/>
+      <c r="AFF33" s="19"/>
+      <c r="AFG33" s="19"/>
+      <c r="AFH33" s="19"/>
+      <c r="AFI33" s="19"/>
+      <c r="AFJ33" s="19"/>
+      <c r="AFK33" s="19"/>
+      <c r="AFL33" s="19"/>
+      <c r="AFM33" s="19"/>
+      <c r="AFN33" s="19"/>
+      <c r="AFO33" s="19"/>
+      <c r="AFP33" s="19"/>
+      <c r="AFQ33" s="19"/>
+      <c r="AFR33" s="19"/>
+      <c r="AFS33" s="19"/>
+      <c r="AFT33" s="19"/>
+      <c r="AFU33" s="19"/>
+      <c r="AFV33" s="19"/>
+      <c r="AFW33" s="19"/>
+      <c r="AFX33" s="19"/>
+      <c r="AFY33" s="19"/>
+      <c r="AFZ33" s="19"/>
+      <c r="AGA33" s="19"/>
+      <c r="AGB33" s="19"/>
+      <c r="AGC33" s="19"/>
+      <c r="AGD33" s="19"/>
+      <c r="AGE33" s="19"/>
+      <c r="AGF33" s="19"/>
+      <c r="AGG33" s="19"/>
+      <c r="AGH33" s="19"/>
+      <c r="AGI33" s="19"/>
+      <c r="AGJ33" s="19"/>
+      <c r="AGK33" s="19"/>
+      <c r="AGL33" s="19"/>
+      <c r="AGM33" s="19"/>
+      <c r="AGN33" s="19"/>
+      <c r="AGO33" s="19"/>
+      <c r="AGP33" s="19"/>
+      <c r="AGQ33" s="19"/>
+      <c r="AGR33" s="19"/>
+      <c r="AGS33" s="19"/>
+      <c r="AGT33" s="19"/>
+      <c r="AGU33" s="19"/>
+      <c r="AGV33" s="19"/>
+      <c r="AGW33" s="19"/>
+      <c r="AGX33" s="19"/>
+      <c r="AGY33" s="19"/>
+      <c r="AGZ33" s="19"/>
+      <c r="AHA33" s="19"/>
+      <c r="AHB33" s="19"/>
+      <c r="AHC33" s="19"/>
+      <c r="AHD33" s="19"/>
+      <c r="AHE33" s="19"/>
+      <c r="AHF33" s="19"/>
+      <c r="AHG33" s="19"/>
+      <c r="AHH33" s="19"/>
+      <c r="AHI33" s="19"/>
+      <c r="AHJ33" s="19"/>
+      <c r="AHK33" s="19"/>
+      <c r="AHL33" s="19"/>
+      <c r="AHM33" s="19"/>
+      <c r="AHN33" s="19"/>
+      <c r="AHO33" s="19"/>
+      <c r="AHP33" s="19"/>
+      <c r="AHQ33" s="19"/>
+      <c r="AHR33" s="19"/>
+      <c r="AHS33" s="19"/>
+      <c r="AHT33" s="19"/>
+      <c r="AHU33" s="19"/>
+      <c r="AHV33" s="19"/>
+      <c r="AHW33" s="19"/>
+      <c r="AHX33" s="19"/>
+      <c r="AHY33" s="19"/>
+      <c r="AHZ33" s="19"/>
+      <c r="AIA33" s="19"/>
+      <c r="AIB33" s="19"/>
+      <c r="AIC33" s="19"/>
+      <c r="AID33" s="19"/>
+      <c r="AIE33" s="19"/>
+      <c r="AIF33" s="19"/>
+      <c r="AIG33" s="19"/>
+      <c r="AIH33" s="19"/>
+      <c r="AII33" s="19"/>
+      <c r="AIJ33" s="19"/>
+      <c r="AIK33" s="19"/>
+      <c r="AIL33" s="19"/>
+      <c r="AIM33" s="19"/>
+      <c r="AIN33" s="19"/>
+      <c r="AIO33" s="19"/>
+      <c r="AIP33" s="19"/>
+      <c r="AIQ33" s="19"/>
+      <c r="AIR33" s="19"/>
+      <c r="AIS33" s="19"/>
+      <c r="AIT33" s="19"/>
+      <c r="AIU33" s="19"/>
+      <c r="AIV33" s="19"/>
+      <c r="AIW33" s="19"/>
+      <c r="AIX33" s="19"/>
+      <c r="AIY33" s="19"/>
+      <c r="AIZ33" s="19"/>
+      <c r="AJA33" s="19"/>
+      <c r="AJB33" s="19"/>
+      <c r="AJC33" s="19"/>
+      <c r="AJD33" s="19"/>
+      <c r="AJE33" s="19"/>
+      <c r="AJF33" s="19"/>
+      <c r="AJG33" s="19"/>
+      <c r="AJH33" s="19"/>
+      <c r="AJI33" s="19"/>
+      <c r="AJJ33" s="19"/>
+      <c r="AJK33" s="19"/>
+      <c r="AJL33" s="19"/>
+      <c r="AJM33" s="19"/>
+      <c r="AJN33" s="19"/>
+      <c r="AJO33" s="19"/>
+      <c r="AJP33" s="19"/>
+      <c r="AJQ33" s="19"/>
+      <c r="AJR33" s="19"/>
+      <c r="AJS33" s="19"/>
+      <c r="AJT33" s="19"/>
+      <c r="AJU33" s="19"/>
+      <c r="AJV33" s="19"/>
+      <c r="AJW33" s="19"/>
+      <c r="AJX33" s="19"/>
+      <c r="AJY33" s="19"/>
+      <c r="AJZ33" s="19"/>
+      <c r="AKA33" s="19"/>
+      <c r="AKB33" s="19"/>
+      <c r="AKC33" s="19"/>
+      <c r="AKD33" s="19"/>
+      <c r="AKE33" s="19"/>
+      <c r="AKF33" s="19"/>
+      <c r="AKG33" s="19"/>
+      <c r="AKH33" s="19"/>
+      <c r="AKI33" s="19"/>
+      <c r="AKJ33" s="19"/>
+      <c r="AKK33" s="19"/>
+      <c r="AKL33" s="19"/>
+      <c r="AKM33" s="19"/>
+      <c r="AKN33" s="19"/>
+      <c r="AKO33" s="19"/>
+      <c r="AKP33" s="19"/>
+      <c r="AKQ33" s="19"/>
+      <c r="AKR33" s="19"/>
+      <c r="AKS33" s="19"/>
+      <c r="AKT33" s="19"/>
+      <c r="AKU33" s="19"/>
+      <c r="AKV33" s="19"/>
+      <c r="AKW33" s="19"/>
+      <c r="AKX33" s="19"/>
+      <c r="AKY33" s="19"/>
+      <c r="AKZ33" s="19"/>
+      <c r="ALA33" s="19"/>
+      <c r="ALB33" s="19"/>
+      <c r="ALC33" s="19"/>
+      <c r="ALD33" s="19"/>
+      <c r="ALE33" s="19"/>
+      <c r="ALF33" s="19"/>
+      <c r="ALG33" s="19"/>
+      <c r="ALH33" s="19"/>
+      <c r="ALI33" s="19"/>
+      <c r="ALJ33" s="19"/>
+      <c r="ALK33" s="19"/>
+      <c r="ALL33" s="19"/>
+      <c r="ALM33" s="19"/>
+      <c r="ALN33" s="19"/>
+      <c r="ALO33" s="19"/>
+      <c r="ALP33" s="19"/>
+      <c r="ALQ33" s="19"/>
+      <c r="ALR33" s="19"/>
+      <c r="ALS33" s="19"/>
+      <c r="ALT33" s="19"/>
+      <c r="ALU33" s="19"/>
+      <c r="ALV33" s="19"/>
+      <c r="ALW33" s="19"/>
+      <c r="ALX33" s="19"/>
+      <c r="ALY33" s="19"/>
+      <c r="ALZ33" s="19"/>
+      <c r="AMA33" s="19"/>
+      <c r="AMB33" s="19"/>
+      <c r="AMC33" s="19"/>
+      <c r="AMD33" s="19"/>
+      <c r="AME33" s="19"/>
+      <c r="AMF33" s="19"/>
+      <c r="AMG33" s="19"/>
+      <c r="AMH33" s="19"/>
+      <c r="AMI33" s="19"/>
+      <c r="AMJ33" s="19"/>
+      <c r="AMK33" s="19"/>
+      <c r="AML33" s="19"/>
+      <c r="AMM33" s="19"/>
+      <c r="AMN33" s="19"/>
+      <c r="AMO33" s="19"/>
+      <c r="AMP33" s="19"/>
+      <c r="AMQ33" s="19"/>
+      <c r="AMR33" s="19"/>
+    </row>
+    <row r="34" spans="1:1032" x14ac:dyDescent="0.3">
+      <c r="B34" s="11"/>
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
@@ -15041,7 +15045,7 @@
       <c r="BX34" s="3"/>
       <c r="BY34" s="3"/>
     </row>
-    <row r="35" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
@@ -15095,7 +15099,7 @@
       <c r="BX35" s="3"/>
       <c r="BY35" s="3"/>
     </row>
-    <row r="36" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
@@ -15149,7 +15153,7 @@
       <c r="BX36" s="3"/>
       <c r="BY36" s="3"/>
     </row>
-    <row r="37" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z37" s="3"/>
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
@@ -15203,7 +15207,7 @@
       <c r="BX37" s="3"/>
       <c r="BY37" s="3"/>
     </row>
-    <row r="38" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
@@ -15257,7 +15261,7 @@
       <c r="BX38" s="3"/>
       <c r="BY38" s="3"/>
     </row>
-    <row r="39" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
@@ -15311,7 +15315,7 @@
       <c r="BX39" s="3"/>
       <c r="BY39" s="3"/>
     </row>
-    <row r="40" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
@@ -15365,7 +15369,7 @@
       <c r="BX40" s="3"/>
       <c r="BY40" s="3"/>
     </row>
-    <row r="41" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
       <c r="AB41" s="3"/>
@@ -15419,7 +15423,7 @@
       <c r="BX41" s="3"/>
       <c r="BY41" s="3"/>
     </row>
-    <row r="42" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z42" s="3"/>
       <c r="AA42" s="3"/>
       <c r="AB42" s="3"/>
@@ -15473,7 +15477,7 @@
       <c r="BX42" s="3"/>
       <c r="BY42" s="3"/>
     </row>
-    <row r="43" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z43" s="3"/>
       <c r="AA43" s="3"/>
       <c r="AB43" s="3"/>
@@ -15527,7 +15531,7 @@
       <c r="BX43" s="3"/>
       <c r="BY43" s="3"/>
     </row>
-    <row r="44" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z44" s="3"/>
       <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
@@ -15581,7 +15585,7 @@
       <c r="BX44" s="3"/>
       <c r="BY44" s="3"/>
     </row>
-    <row r="45" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z45" s="3"/>
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
@@ -15635,7 +15639,7 @@
       <c r="BX45" s="3"/>
       <c r="BY45" s="3"/>
     </row>
-    <row r="46" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z46" s="3"/>
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
@@ -15689,7 +15693,7 @@
       <c r="BX46" s="3"/>
       <c r="BY46" s="3"/>
     </row>
-    <row r="47" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z47" s="3"/>
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
@@ -15743,7 +15747,7 @@
       <c r="BX47" s="3"/>
       <c r="BY47" s="3"/>
     </row>
-    <row r="48" spans="2:77" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1032" x14ac:dyDescent="0.3">
       <c r="Z48" s="3"/>
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
@@ -43553,6 +43557,60 @@
       <c r="BX562" s="3"/>
       <c r="BY562" s="3"/>
     </row>
+    <row r="563" spans="26:77" x14ac:dyDescent="0.3">
+      <c r="Z563" s="3"/>
+      <c r="AA563" s="3"/>
+      <c r="AB563" s="3"/>
+      <c r="AC563" s="3"/>
+      <c r="AD563" s="3"/>
+      <c r="AE563" s="3"/>
+      <c r="AF563" s="3"/>
+      <c r="AG563" s="3"/>
+      <c r="AH563" s="3"/>
+      <c r="AI563" s="3"/>
+      <c r="AJ563" s="3"/>
+      <c r="AK563" s="3"/>
+      <c r="AL563" s="3"/>
+      <c r="AM563" s="3"/>
+      <c r="AN563" s="3"/>
+      <c r="AO563" s="3"/>
+      <c r="AP563" s="3"/>
+      <c r="AQ563" s="3"/>
+      <c r="AR563" s="3"/>
+      <c r="AS563" s="3"/>
+      <c r="AT563" s="3"/>
+      <c r="AU563" s="3"/>
+      <c r="AV563" s="3"/>
+      <c r="AW563" s="3"/>
+      <c r="AX563" s="3"/>
+      <c r="AY563" s="3"/>
+      <c r="AZ563" s="3"/>
+      <c r="BA563" s="3"/>
+      <c r="BB563" s="3"/>
+      <c r="BC563" s="3"/>
+      <c r="BD563" s="3"/>
+      <c r="BE563" s="3"/>
+      <c r="BF563" s="3"/>
+      <c r="BG563" s="3"/>
+      <c r="BH563" s="3"/>
+      <c r="BI563" s="3"/>
+      <c r="BJ563" s="3"/>
+      <c r="BK563" s="3"/>
+      <c r="BL563" s="3"/>
+      <c r="BM563" s="3"/>
+      <c r="BN563" s="3"/>
+      <c r="BO563" s="3"/>
+      <c r="BP563" s="3"/>
+      <c r="BQ563" s="3"/>
+      <c r="BR563" s="3"/>
+      <c r="BS563" s="3"/>
+      <c r="BT563" s="3"/>
+      <c r="BU563" s="3"/>
+      <c r="BV563" s="3"/>
+      <c r="BW563" s="3"/>
+      <c r="BX563" s="3"/>
+      <c r="BY563" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="R17:U17"/>
@@ -43563,7 +43621,7 @@
     <mergeCell ref="F17:I17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1"/>
+    <hyperlink ref="A30" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -43586,33 +43644,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.25" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.25" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="58"/>
+    <col min="1" max="1" width="15.25" style="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.25" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="53"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
-        <v>11</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
+        <v>16</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>20</v>
+      <c r="B4" s="53" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP authority stats with postcodes
</commit_message>
<xml_diff>
--- a/scripts/cli/authority_stats.xlsx
+++ b/scripts/cli/authority_stats.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Standard report" sheetId="1" r:id="rId1"/>
-    <sheet name="Notes" sheetId="2" r:id="rId2"/>
+    <sheet name="Postcode breakdown" sheetId="3" r:id="rId2"/>
+    <sheet name="Notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -246,6 +247,30 @@
   </si>
   <si>
     <t>Calculated using WRAP's Benefits of Reuse tool.</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Number of confirmed gifts made</t>
+  </si>
+  <si>
+    <t>Searches</t>
+  </si>
+  <si>
+    <t>CO2 (kg)</t>
+  </si>
+  <si>
+    <t>OFFERs made</t>
+  </si>
+  <si>
+    <t>WANTEDs made</t>
+  </si>
+  <si>
+    <t>Gifts made</t>
+  </si>
+  <si>
+    <t>Weight of gifts made (kg)</t>
   </si>
 </sst>
 </file>
@@ -1268,13 +1293,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR563"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="2" customWidth="1"/>
     <col min="2" max="25" width="8.5" style="2" customWidth="1"/>
     <col min="26" max="75" width="8.5" style="5" customWidth="1"/>
     <col min="76" max="1032" width="8.5" style="2" customWidth="1"/>
@@ -7901,7 +7926,7 @@
     </row>
     <row r="13" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -43636,6 +43661,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+    <col min="6" max="6" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Remove unused tab in authority_stats.xlsx
</commit_message>
<xml_diff>
--- a/scripts/cli/authority_stats.xlsx
+++ b/scripts/cli/authority_stats.xlsx
@@ -14,7 +14,6 @@
   <sheets>
     <sheet name="Standard report" sheetId="1" r:id="rId1"/>
     <sheet name="Postcode breakdown" sheetId="3" r:id="rId2"/>
-    <sheet name="Notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -175,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -243,12 +242,6 @@
     <t>The full data associated with any shortlinks can be viewed by clicking  the link below and then scrolling to the appropriate shortlink.</t>
   </si>
   <si>
-    <t>Current total number of Freeglers</t>
-  </si>
-  <si>
-    <t>Calculated using WRAP's Benefits of Reuse tool.</t>
-  </si>
-  <si>
     <t>Postcode</t>
   </si>
   <si>
@@ -283,7 +276,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,26 +499,6 @@
       <i/>
       <sz val="9"/>
       <color rgb="FF0070C0"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -758,7 +731,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -860,9 +833,6 @@
     <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1712,12 +1682,12 @@
     </row>
     <row r="7" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -7926,7 +7896,7 @@
     </row>
     <row r="13" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -9058,39 +9028,39 @@
     </row>
     <row r="17" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="70" t="s">
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="65" t="s">
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="65" t="s">
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="65"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="65" t="s">
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="S17" s="65"/>
-      <c r="T17" s="65"/>
-      <c r="U17" s="66"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="63"/>
     </row>
     <row r="18" spans="1:1032" s="20" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="31">
@@ -9467,7 +9437,7 @@
       <c r="BY22" s="15"/>
     </row>
     <row r="23" spans="1:1032" s="39" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="53" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="13"/>
@@ -9548,17 +9518,17 @@
       <c r="BY23" s="15"/>
     </row>
     <row r="24" spans="1:1032" s="40" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A24" s="64"/>
-      <c r="B24" s="62">
+      <c r="A24" s="61"/>
+      <c r="B24" s="59">
         <v>43466</v>
       </c>
-      <c r="C24" s="57">
+      <c r="C24" s="54">
         <v>43497</v>
       </c>
-      <c r="D24" s="57">
+      <c r="D24" s="54">
         <v>43525</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="55" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="19"/>
@@ -9635,11 +9605,11 @@
       <c r="BY24" s="15"/>
     </row>
     <row r="25" spans="1:1032" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="15"/>
       <c r="AI25" s="15"/>
@@ -43664,7 +43634,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -43676,25 +43646,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
@@ -43718,49 +43688,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.25" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.25" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="53"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>